<commit_message>
Minor updates to templates
</commit_message>
<xml_diff>
--- a/templates/NOMADS_Library_Rapid_Worksheet.xlsx
+++ b/templates/NOMADS_Library_Rapid_Worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\warehouse\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BDB9A9-F5D1-4B9B-956D-E9D6DC780629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5B4B05-1243-4E9E-9D50-4E25570CDEE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="34080" windowHeight="22200" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="403">
   <si>
     <t>Date:</t>
   </si>
@@ -1478,11 +1478,41 @@
     <t>Person C</t>
   </si>
   <si>
-    <t>2. Clean up: Add 0.5x vol AMPPure beads, 5 min RT with mixing, wash with fresh 80% EtOH, spin, dry, re-suspend in 15 µl EB (10 min @RT) and transfer eluate to fresh tube</t>
+    <t>4 - Loading Library</t>
+  </si>
+  <si>
+    <t>Volume of EB to add (µll)</t>
+  </si>
+  <si>
+    <t>2. Add 1 µl of diluted RA + ADB to the 10 µl of adapter ligated cleaned pooled DNA</t>
+  </si>
+  <si>
+    <t>Sequencing Buffer (SB)</t>
+  </si>
+  <si>
+    <t>Loading Beads (LIB)</t>
+  </si>
+  <si>
+    <t>Sample Type</t>
+  </si>
+  <si>
+    <t>sample_type</t>
+  </si>
+  <si>
+    <t>Added Sample type</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>Negative</t>
   </si>
   <si>
     <r>
-      <t>3. Quantify 1 µl of a 1:10 dilution (NF H</t>
+      <t>3. Quantify 2 µl of a 1:10 dilution (NF H</t>
     </r>
     <r>
       <rPr>
@@ -1502,41 +1532,8 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>O ) of the DNA  (199 µl WS 1X HS DNA) on Qubit</t>
+      <t>O ) of the DNA  (198 µl WS 1X HS DNA) on Qubit</t>
     </r>
-  </si>
-  <si>
-    <t>4 - Loading Library</t>
-  </si>
-  <si>
-    <t>Volume of EB to add (µll)</t>
-  </si>
-  <si>
-    <t>2. Add 1 µl of diluted RA + ADB to the 10 µl of adapter ligated cleaned pooled DNA</t>
-  </si>
-  <si>
-    <t>Sequencing Buffer (SB)</t>
-  </si>
-  <si>
-    <t>Loading Beads (LIB)</t>
-  </si>
-  <si>
-    <t>Sample Type</t>
-  </si>
-  <si>
-    <t>sample_type</t>
-  </si>
-  <si>
-    <t>Added Sample type</t>
-  </si>
-  <si>
-    <t>Field</t>
-  </si>
-  <si>
-    <t>Positive</t>
-  </si>
-  <si>
-    <t>Negative</t>
   </si>
 </sst>
 </file>
@@ -2156,7 +2153,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2425,47 +2422,80 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2486,44 +2516,32 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -2903,6 +2921,7 @@
       <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -2977,7 +2996,7 @@
         <vertical/>
         <horizontal/>
       </border>
-      <protection locked="0" hidden="0"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -3408,8 +3427,8 @@
   </sheetPr>
   <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:F4"/>
+    <sheetView topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3418,204 +3437,206 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="119" t="s">
         <v>371</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
-      <c r="F1" s="89"/>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
-      <c r="J1" s="89"/>
-      <c r="K1" s="89"/>
-      <c r="L1" s="89"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
+      <c r="H1" s="119"/>
+      <c r="I1" s="119"/>
+      <c r="J1" s="119"/>
+      <c r="K1" s="119"/>
+      <c r="L1" s="119"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="90" t="s">
+      <c r="A2" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="90"/>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="92" t="s">
+      <c r="B2" s="94"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="120"/>
+      <c r="G2" s="101" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="92"/>
-      <c r="J2" s="93" t="s">
+      <c r="H2" s="101"/>
+      <c r="J2" s="121" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="93"/>
+      <c r="K2" s="121"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="90"/>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="94"/>
-      <c r="F3" s="94"/>
+      <c r="B3" s="94"/>
+      <c r="C3" s="122"/>
+      <c r="D3" s="122"/>
+      <c r="E3" s="122"/>
+      <c r="F3" s="122"/>
       <c r="G3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="95" t="s">
+      <c r="J3" s="123" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="95"/>
+      <c r="K3" s="123"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="90" t="s">
+      <c r="A4" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="90"/>
-      <c r="C4" s="91"/>
-      <c r="D4" s="91"/>
-      <c r="E4" s="91"/>
-      <c r="F4" s="91"/>
+      <c r="B4" s="94"/>
+      <c r="C4" s="120"/>
+      <c r="D4" s="120"/>
+      <c r="E4" s="120"/>
+      <c r="F4" s="120"/>
       <c r="G4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="96" t="s">
+      <c r="J4" s="124" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="96"/>
+      <c r="K4" s="124"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="97" t="s">
+      <c r="A5" s="110" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="97"/>
-      <c r="C5" s="98" t="str">
+      <c r="B5" s="110"/>
+      <c r="C5" s="108" t="str">
         <f>IF(OR(ISBLANK(C3),ISBLANK(C4)),"",CONCATENATE("SL",VLOOKUP(C3,reference!H3:I9,2,FALSE()),C4))</f>
         <v/>
       </c>
-      <c r="D5" s="98"/>
-      <c r="E5" s="98"/>
-      <c r="F5" s="98"/>
+      <c r="D5" s="108"/>
+      <c r="E5" s="108"/>
+      <c r="F5" s="108"/>
       <c r="G5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="99" t="s">
+      <c r="J5" s="109" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="99"/>
+      <c r="K5" s="109"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="97" t="s">
+      <c r="A6" s="110" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="97"/>
-      <c r="C6" s="100" t="str">
+      <c r="B6" s="110"/>
+      <c r="C6" s="111" t="str">
         <f>IF(OR(ISBLANK(C2),ISBLANK(C3),ISBLANK(C4)),"",CONCATENATE(C2,"_SeqLib_",C5))</f>
         <v/>
       </c>
-      <c r="D6" s="100"/>
-      <c r="E6" s="100"/>
-      <c r="F6" s="100"/>
+      <c r="D6" s="111"/>
+      <c r="E6" s="111"/>
+      <c r="F6" s="111"/>
       <c r="G6" s="4"/>
-      <c r="J6" s="99"/>
-      <c r="K6" s="99"/>
+      <c r="J6" s="109"/>
+      <c r="K6" s="109"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="87" t="s">
+      <c r="A7" s="117" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="87"/>
-      <c r="C7" s="88"/>
-      <c r="D7" s="88"/>
-      <c r="E7" s="88"/>
-      <c r="F7" s="88"/>
+      <c r="B7" s="117"/>
+      <c r="C7" s="118"/>
+      <c r="D7" s="118"/>
+      <c r="E7" s="118"/>
+      <c r="F7" s="118"/>
       <c r="G7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="87" t="s">
+      <c r="A8" s="117" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="87"/>
-      <c r="C8" s="88"/>
-      <c r="D8" s="88"/>
-      <c r="E8" s="88"/>
-      <c r="F8" s="88"/>
+      <c r="B8" s="117"/>
+      <c r="C8" s="118"/>
+      <c r="D8" s="118"/>
+      <c r="E8" s="118"/>
+      <c r="F8" s="118"/>
       <c r="G8" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="102" t="s">
+      <c r="A9" s="113" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="102"/>
-      <c r="C9" s="103" t="str">
+      <c r="B9" s="113"/>
+      <c r="C9" s="114" t="str">
         <f>IF(OR(LEN(C7)=0, LEN(C8)=0),"",CONCATENATE(C7,"_Batch",C8))</f>
         <v/>
       </c>
-      <c r="D9" s="103"/>
-      <c r="E9" s="103"/>
-      <c r="F9" s="103"/>
+      <c r="D9" s="114"/>
+      <c r="E9" s="114"/>
+      <c r="F9" s="114"/>
       <c r="G9" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="102" t="s">
+      <c r="A10" s="113" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="102"/>
-      <c r="C10" s="103" t="str">
+      <c r="B10" s="113"/>
+      <c r="C10" s="114" t="str">
         <f>IF(OR(LEN(C6)=0,LEN(exp_summary)=0),"",CONCATENATE(C6,"_",exp_summary))</f>
         <v/>
       </c>
-      <c r="D10" s="103"/>
-      <c r="E10" s="103"/>
-      <c r="F10" s="103"/>
-      <c r="G10" s="103"/>
-      <c r="H10" s="103"/>
+      <c r="D10" s="114"/>
+      <c r="E10" s="114"/>
+      <c r="F10" s="114"/>
+      <c r="G10" s="114"/>
+      <c r="H10" s="114"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="90" t="s">
+      <c r="A11" s="94" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="90"/>
-      <c r="C11" s="26"/>
+      <c r="B11" s="94"/>
+      <c r="C11" s="26">
+        <v>10</v>
+      </c>
       <c r="D11" s="24"/>
       <c r="E11" s="24"/>
       <c r="F11" s="24"/>
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="90" t="s">
+      <c r="A12" s="94" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="90"/>
-      <c r="C12" s="104"/>
-      <c r="D12" s="104"/>
-      <c r="E12" s="104"/>
-      <c r="F12" s="104"/>
-      <c r="G12" s="104"/>
-      <c r="H12" s="104"/>
-      <c r="I12" s="104"/>
-      <c r="J12" s="104"/>
-      <c r="K12" s="104"/>
+      <c r="B12" s="94"/>
+      <c r="C12" s="115"/>
+      <c r="D12" s="115"/>
+      <c r="E12" s="115"/>
+      <c r="F12" s="115"/>
+      <c r="G12" s="115"/>
+      <c r="H12" s="115"/>
+      <c r="I12" s="115"/>
+      <c r="J12" s="115"/>
+      <c r="K12" s="115"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="104"/>
-      <c r="D13" s="104"/>
-      <c r="E13" s="104"/>
-      <c r="F13" s="104"/>
-      <c r="G13" s="104"/>
-      <c r="H13" s="104"/>
-      <c r="I13" s="104"/>
-      <c r="J13" s="104"/>
-      <c r="K13" s="104"/>
+      <c r="C13" s="115"/>
+      <c r="D13" s="115"/>
+      <c r="E13" s="115"/>
+      <c r="F13" s="115"/>
+      <c r="G13" s="115"/>
+      <c r="H13" s="115"/>
+      <c r="I13" s="115"/>
+      <c r="J13" s="115"/>
+      <c r="K13" s="115"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C14" s="5"/>
@@ -3630,19 +3651,19 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="str">
-        <f>_xlfn.CONCAT("1. Add ", pcr_product_targetmass_per_sample, " ng sample PCR product into a fresh plate according to concentration")</f>
-        <v>1. Add 200 ng sample PCR product into a fresh plate according to concentration</v>
+        <f>_xlfn.CONCAT("1. Add ", pcr_product_targetmass_per_sample, " ng of clean PCR product into a fresh plate according to concentration.")</f>
+        <v>1. Add 200 ng of clean PCR product into a fresh plate according to concentration.</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="H16" s="4"/>
-      <c r="I16" s="105" t="s">
+      <c r="I16" s="116" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="105"/>
-      <c r="K16" s="105"/>
+      <c r="J16" s="116"/>
+      <c r="K16" s="116"/>
     </row>
     <row r="17" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
@@ -3653,10 +3674,10 @@
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="G17" s="8"/>
-      <c r="I17" s="106" t="s">
+      <c r="I17" s="98" t="s">
         <v>25</v>
       </c>
-      <c r="J17" s="106"/>
+      <c r="J17" s="98"/>
       <c r="K17" s="9" t="s">
         <v>26</v>
       </c>
@@ -3668,10 +3689,10 @@
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="G18" s="8"/>
-      <c r="I18" s="101">
+      <c r="I18" s="112">
         <v>30</v>
       </c>
-      <c r="J18" s="101"/>
+      <c r="J18" s="112"/>
       <c r="K18" s="2" t="s">
         <v>27</v>
       </c>
@@ -3683,10 +3704,10 @@
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="G19" s="8"/>
-      <c r="I19" s="101">
+      <c r="I19" s="112">
         <v>30</v>
       </c>
-      <c r="J19" s="101"/>
+      <c r="J19" s="112"/>
       <c r="K19" s="7">
         <v>2</v>
       </c>
@@ -3698,10 +3719,10 @@
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="G20" s="8"/>
-      <c r="I20" s="101">
+      <c r="I20" s="112">
         <v>80</v>
       </c>
-      <c r="J20" s="101"/>
+      <c r="J20" s="112"/>
       <c r="K20" s="2">
         <v>2</v>
       </c>
@@ -3713,10 +3734,10 @@
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="G21" s="8"/>
-      <c r="I21" s="101">
+      <c r="I21" s="112">
         <v>8</v>
       </c>
-      <c r="J21" s="101"/>
+      <c r="J21" s="112"/>
       <c r="K21" s="2" t="s">
         <v>27</v>
       </c>
@@ -3739,24 +3760,25 @@
       <c r="G23" s="25"/>
     </row>
     <row r="24" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="92" t="s">
-        <v>391</v>
-      </c>
-      <c r="B24" s="92"/>
-      <c r="C24" s="92"/>
-      <c r="D24" s="92"/>
-      <c r="E24" s="92"/>
-      <c r="F24" s="92"/>
-      <c r="G24" s="92"/>
-      <c r="H24" s="92"/>
-      <c r="I24" s="92"/>
-      <c r="J24" s="92"/>
-      <c r="K24" s="92"/>
-      <c r="L24" s="92"/>
+      <c r="A24" s="101" t="str">
+        <f>_xlfn.CONCAT("2. Clean up: Add 0.5x vol (", SUM(5*exp_rxns)*0.5,"µl) AMPPure beads for 5 min RT with mixing, wash with fresh 80% EtOH, spin, dry, re-suspend in 15 µl EB (10 min @RT) and transfer eluate to fresh tube")</f>
+        <v>2. Clean up: Add 0.5x vol (25µl) AMPPure beads for 5 min RT with mixing, wash with fresh 80% EtOH, spin, dry, re-suspend in 15 µl EB (10 min @RT) and transfer eluate to fresh tube</v>
+      </c>
+      <c r="B24" s="101"/>
+      <c r="C24" s="101"/>
+      <c r="D24" s="101"/>
+      <c r="E24" s="101"/>
+      <c r="F24" s="101"/>
+      <c r="G24" s="101"/>
+      <c r="H24" s="101"/>
+      <c r="I24" s="101"/>
+      <c r="J24" s="101"/>
+      <c r="K24" s="101"/>
+      <c r="L24" s="101"/>
     </row>
     <row r="25" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>392</v>
+        <v>402</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -3775,43 +3797,43 @@
       <c r="C26" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="109" t="s">
+      <c r="D26" s="102" t="s">
         <v>32</v>
       </c>
-      <c r="E26" s="109"/>
-      <c r="F26" s="112" t="s">
+      <c r="E26" s="102"/>
+      <c r="F26" s="105" t="s">
         <v>388</v>
       </c>
-      <c r="G26" s="112"/>
-      <c r="H26" s="112" t="s">
-        <v>394</v>
-      </c>
-      <c r="I26" s="112"/>
+      <c r="G26" s="105"/>
+      <c r="H26" s="105" t="s">
+        <v>392</v>
+      </c>
+      <c r="I26" s="105"/>
     </row>
     <row r="27" spans="1:17" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <f>SUM(exp_rxns*5)*0.5</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B27" s="31"/>
       <c r="C27" s="31">
         <v>10</v>
       </c>
-      <c r="D27" s="110">
+      <c r="D27" s="103">
         <f>SUM(B27*C27)</f>
         <v>0</v>
       </c>
-      <c r="E27" s="110"/>
-      <c r="F27" s="111" t="str">
+      <c r="E27" s="103"/>
+      <c r="F27" s="104" t="str">
         <f>IFERROR(IF(SUM(flowcell_targetmass/DNAconc_pooled)&gt;flowcell_maxvol-1,flowcell_maxvol-1, SUM(flowcell_targetmass/DNAconc_pooled)),"")</f>
         <v/>
       </c>
-      <c r="G27" s="111"/>
-      <c r="H27" s="111" t="str">
+      <c r="G27" s="104"/>
+      <c r="H27" s="104" t="str">
         <f>IFERROR(SUM(10-F27),"")</f>
         <v/>
       </c>
-      <c r="I27" s="111"/>
+      <c r="I27" s="104"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
@@ -3828,7 +3850,7 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
@@ -3844,52 +3866,52 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="106" t="s">
+      <c r="A35" s="98" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="106"/>
-      <c r="C35" s="106"/>
-      <c r="D35" s="113" t="s">
+      <c r="B35" s="98"/>
+      <c r="C35" s="98"/>
+      <c r="D35" s="106" t="s">
         <v>24</v>
       </c>
-      <c r="E35" s="113"/>
+      <c r="E35" s="106"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="109" t="s">
+      <c r="A36" s="102" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="109"/>
-      <c r="C36" s="109"/>
-      <c r="D36" s="114">
+      <c r="B36" s="102"/>
+      <c r="C36" s="102"/>
+      <c r="D36" s="107">
         <v>11</v>
       </c>
-      <c r="E36" s="114"/>
+      <c r="E36" s="107"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="107" t="s">
-        <v>396</v>
-      </c>
-      <c r="B37" s="107"/>
-      <c r="C37" s="107"/>
-      <c r="D37" s="108">
+      <c r="A37" s="99" t="s">
+        <v>394</v>
+      </c>
+      <c r="B37" s="99"/>
+      <c r="C37" s="99"/>
+      <c r="D37" s="100">
         <v>37.5</v>
       </c>
-      <c r="E37" s="108"/>
+      <c r="E37" s="100"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="107" t="s">
-        <v>397</v>
-      </c>
-      <c r="B38" s="107"/>
-      <c r="C38" s="107"/>
-      <c r="D38" s="108">
+      <c r="A38" s="99" t="s">
+        <v>395</v>
+      </c>
+      <c r="B38" s="99"/>
+      <c r="C38" s="99"/>
+      <c r="D38" s="100">
         <v>25.5</v>
       </c>
-      <c r="E38" s="108"/>
+      <c r="E38" s="100"/>
       <c r="F38" s="4" t="s">
         <v>35</v>
       </c>
@@ -3901,75 +3923,75 @@
       <c r="C40" s="4"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="90" t="s">
+      <c r="A41" s="94" t="s">
         <v>37</v>
       </c>
-      <c r="B41" s="90"/>
-      <c r="C41" s="116"/>
-      <c r="D41" s="116"/>
+      <c r="B41" s="94"/>
+      <c r="C41" s="96"/>
+      <c r="D41" s="96"/>
       <c r="E41" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="90" t="s">
+      <c r="A42" s="94" t="s">
         <v>39</v>
       </c>
-      <c r="B42" s="90"/>
-      <c r="C42" s="115"/>
-      <c r="D42" s="115"/>
+      <c r="B42" s="94"/>
+      <c r="C42" s="95"/>
+      <c r="D42" s="95"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="90" t="s">
+      <c r="A43" s="94" t="s">
         <v>40</v>
       </c>
-      <c r="B43" s="90"/>
-      <c r="C43" s="115"/>
-      <c r="D43" s="115"/>
+      <c r="B43" s="94"/>
+      <c r="C43" s="95"/>
+      <c r="D43" s="95"/>
     </row>
     <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="90" t="s">
+      <c r="A44" s="94" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="90"/>
-      <c r="C44" s="117" t="str">
+      <c r="B44" s="94"/>
+      <c r="C44" s="97" t="str">
         <f>IF(flowcell_status="New",0,"")</f>
         <v/>
       </c>
-      <c r="D44" s="117"/>
+      <c r="D44" s="97"/>
       <c r="E44" s="8" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="90" t="s">
+      <c r="A45" s="94" t="s">
         <v>43</v>
       </c>
-      <c r="B45" s="90"/>
-      <c r="C45" s="116"/>
-      <c r="D45" s="116"/>
+      <c r="B45" s="94"/>
+      <c r="C45" s="96"/>
+      <c r="D45" s="96"/>
       <c r="E45" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="90" t="s">
+      <c r="A46" s="94" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="90"/>
-      <c r="C46" s="115"/>
-      <c r="D46" s="115"/>
+      <c r="B46" s="94"/>
+      <c r="C46" s="95"/>
+      <c r="D46" s="95"/>
       <c r="E46" s="8" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="90" t="s">
+      <c r="A47" s="94" t="s">
         <v>47</v>
       </c>
-      <c r="B47" s="90"/>
-      <c r="C47" s="115"/>
-      <c r="D47" s="115"/>
+      <c r="B47" s="94"/>
+      <c r="C47" s="95"/>
+      <c r="D47" s="95"/>
       <c r="E47" s="8" t="s">
         <v>48</v>
       </c>
@@ -3977,20 +3999,38 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="62">
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="J5:K6"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:K13"/>
+    <mergeCell ref="I16:K16"/>
     <mergeCell ref="I17:J17"/>
     <mergeCell ref="A37:C37"/>
     <mergeCell ref="D37:E37"/>
@@ -4007,38 +4047,20 @@
     <mergeCell ref="D36:E36"/>
     <mergeCell ref="H26:I26"/>
     <mergeCell ref="H27:I27"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="J5:K6"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:K13"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="J2:K2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="C45:D45"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:C4 C7:C8 C11:C12 B27:C27 C41:C43 C45:C47">
     <cfRule type="expression" dxfId="6" priority="7">
@@ -4149,7 +4171,7 @@
   <dimension ref="A1:Z111"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4157,8 +4179,7 @@
     <col min="1" max="1" width="5.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.25" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="6.625" customWidth="1"/>
-    <col min="4" max="5" width="11.875" customWidth="1"/>
-    <col min="6" max="6" width="12.625" style="2" customWidth="1"/>
+    <col min="4" max="6" width="11.875" customWidth="1"/>
     <col min="7" max="7" width="13.125" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
     <col min="13" max="22" width="11" hidden="1" customWidth="1"/>
@@ -4166,43 +4187,43 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C1" s="44"/>
-      <c r="D1" s="118" t="s">
+      <c r="D1" s="125" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="118"/>
-      <c r="F1" s="118"/>
+      <c r="E1" s="125"/>
+      <c r="F1" s="125"/>
       <c r="G1" s="68" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="119" t="s">
+      <c r="H1" s="126" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="119"/>
-      <c r="J1" s="119"/>
-      <c r="K1" s="119"/>
-      <c r="L1" s="120" t="s">
+      <c r="I1" s="126"/>
+      <c r="J1" s="126"/>
+      <c r="K1" s="126"/>
+      <c r="L1" s="127" t="s">
         <v>52</v>
       </c>
-      <c r="M1" s="120"/>
-      <c r="N1" s="120"/>
-      <c r="O1" s="120"/>
-      <c r="P1" s="120"/>
-      <c r="Q1" s="120"/>
-      <c r="R1" s="120"/>
-      <c r="S1" s="120"/>
-      <c r="T1" s="120"/>
-      <c r="U1" s="120"/>
-      <c r="V1" s="120"/>
-      <c r="W1" s="120"/>
-      <c r="X1" s="120"/>
-      <c r="Y1" s="120"/>
-      <c r="Z1" s="120"/>
+      <c r="M1" s="127"/>
+      <c r="N1" s="127"/>
+      <c r="O1" s="127"/>
+      <c r="P1" s="127"/>
+      <c r="Q1" s="127"/>
+      <c r="R1" s="127"/>
+      <c r="S1" s="127"/>
+      <c r="T1" s="127"/>
+      <c r="U1" s="127"/>
+      <c r="V1" s="127"/>
+      <c r="W1" s="127"/>
+      <c r="X1" s="127"/>
+      <c r="Y1" s="127"/>
+      <c r="Z1" s="127"/>
     </row>
     <row r="2" spans="1:26" s="10" customFormat="1" ht="81" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="87" t="s">
         <v>332</v>
       </c>
       <c r="C2" s="46" t="s">
@@ -4215,7 +4236,7 @@
         <v>56</v>
       </c>
       <c r="F2" s="69" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G2" s="70" t="s">
         <v>57</v>
@@ -4282,7 +4303,7 @@
       <c r="A3" s="47">
         <v>1</v>
       </c>
-      <c r="B3" s="49" t="str">
+      <c r="B3" s="88" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>1</v>
       </c>
@@ -4361,7 +4382,7 @@
       <c r="A4" s="56">
         <v>2</v>
       </c>
-      <c r="B4" s="29" t="str">
+      <c r="B4" s="89" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>1</v>
       </c>
@@ -4440,7 +4461,7 @@
       <c r="A5" s="56">
         <v>3</v>
       </c>
-      <c r="B5" s="29" t="str">
+      <c r="B5" s="89" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>1</v>
       </c>
@@ -4519,7 +4540,7 @@
       <c r="A6" s="56">
         <v>4</v>
       </c>
-      <c r="B6" s="29" t="str">
+      <c r="B6" s="89" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>1</v>
       </c>
@@ -4598,7 +4619,7 @@
       <c r="A7" s="56">
         <v>5</v>
       </c>
-      <c r="B7" s="29" t="str">
+      <c r="B7" s="89" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>1</v>
       </c>
@@ -4677,7 +4698,7 @@
       <c r="A8" s="56">
         <v>6</v>
       </c>
-      <c r="B8" s="29" t="str">
+      <c r="B8" s="89" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>1</v>
       </c>
@@ -4756,7 +4777,7 @@
       <c r="A9" s="56">
         <v>7</v>
       </c>
-      <c r="B9" s="29" t="str">
+      <c r="B9" s="89" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>1</v>
       </c>
@@ -4835,7 +4856,7 @@
       <c r="A10" s="58">
         <v>8</v>
       </c>
-      <c r="B10" s="62" t="str">
+      <c r="B10" s="90" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>1</v>
       </c>
@@ -4914,7 +4935,7 @@
       <c r="A11" s="73">
         <v>9</v>
       </c>
-      <c r="B11" s="43" t="str">
+      <c r="B11" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>2</v>
       </c>
@@ -4993,7 +5014,7 @@
       <c r="A12" s="56">
         <v>10</v>
       </c>
-      <c r="B12" s="43" t="str">
+      <c r="B12" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>2</v>
       </c>
@@ -5072,7 +5093,7 @@
       <c r="A13" s="56">
         <v>11</v>
       </c>
-      <c r="B13" s="43" t="str">
+      <c r="B13" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>2</v>
       </c>
@@ -5151,7 +5172,7 @@
       <c r="A14" s="56">
         <v>12</v>
       </c>
-      <c r="B14" s="43" t="str">
+      <c r="B14" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>2</v>
       </c>
@@ -5230,7 +5251,7 @@
       <c r="A15" s="56">
         <v>13</v>
       </c>
-      <c r="B15" s="43" t="str">
+      <c r="B15" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>2</v>
       </c>
@@ -5309,7 +5330,7 @@
       <c r="A16" s="56">
         <v>14</v>
       </c>
-      <c r="B16" s="43" t="str">
+      <c r="B16" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>2</v>
       </c>
@@ -5388,7 +5409,7 @@
       <c r="A17" s="56">
         <v>15</v>
       </c>
-      <c r="B17" s="43" t="str">
+      <c r="B17" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>2</v>
       </c>
@@ -5467,7 +5488,7 @@
       <c r="A18" s="58">
         <v>16</v>
       </c>
-      <c r="B18" s="59" t="str">
+      <c r="B18" s="92" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>2</v>
       </c>
@@ -5546,7 +5567,7 @@
       <c r="A19" s="47">
         <v>17</v>
       </c>
-      <c r="B19" s="48" t="str">
+      <c r="B19" s="93" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>3</v>
       </c>
@@ -5625,7 +5646,7 @@
       <c r="A20" s="56">
         <v>18</v>
       </c>
-      <c r="B20" s="43" t="str">
+      <c r="B20" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>3</v>
       </c>
@@ -5704,7 +5725,7 @@
       <c r="A21" s="56">
         <v>19</v>
       </c>
-      <c r="B21" s="43" t="str">
+      <c r="B21" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>3</v>
       </c>
@@ -5783,7 +5804,7 @@
       <c r="A22" s="56">
         <v>20</v>
       </c>
-      <c r="B22" s="43" t="str">
+      <c r="B22" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>3</v>
       </c>
@@ -5862,7 +5883,7 @@
       <c r="A23" s="56">
         <v>21</v>
       </c>
-      <c r="B23" s="43" t="str">
+      <c r="B23" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>3</v>
       </c>
@@ -5941,7 +5962,7 @@
       <c r="A24" s="56">
         <v>22</v>
       </c>
-      <c r="B24" s="43" t="str">
+      <c r="B24" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>3</v>
       </c>
@@ -6020,7 +6041,7 @@
       <c r="A25" s="56">
         <v>23</v>
       </c>
-      <c r="B25" s="43" t="str">
+      <c r="B25" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>3</v>
       </c>
@@ -6099,7 +6120,7 @@
       <c r="A26" s="58">
         <v>24</v>
       </c>
-      <c r="B26" s="59" t="str">
+      <c r="B26" s="92" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>3</v>
       </c>
@@ -6178,7 +6199,7 @@
       <c r="A27" s="47">
         <v>25</v>
       </c>
-      <c r="B27" s="48" t="str">
+      <c r="B27" s="93" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>4</v>
       </c>
@@ -6257,7 +6278,7 @@
       <c r="A28" s="56">
         <v>26</v>
       </c>
-      <c r="B28" s="43" t="str">
+      <c r="B28" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>4</v>
       </c>
@@ -6336,7 +6357,7 @@
       <c r="A29" s="56">
         <v>27</v>
       </c>
-      <c r="B29" s="43" t="str">
+      <c r="B29" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>4</v>
       </c>
@@ -6415,7 +6436,7 @@
       <c r="A30" s="56">
         <v>28</v>
       </c>
-      <c r="B30" s="43" t="str">
+      <c r="B30" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>4</v>
       </c>
@@ -6494,7 +6515,7 @@
       <c r="A31" s="56">
         <v>29</v>
       </c>
-      <c r="B31" s="43" t="str">
+      <c r="B31" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>4</v>
       </c>
@@ -6573,7 +6594,7 @@
       <c r="A32" s="56">
         <v>30</v>
       </c>
-      <c r="B32" s="43" t="str">
+      <c r="B32" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>4</v>
       </c>
@@ -6652,7 +6673,7 @@
       <c r="A33" s="56">
         <v>31</v>
       </c>
-      <c r="B33" s="43" t="str">
+      <c r="B33" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>4</v>
       </c>
@@ -6731,7 +6752,7 @@
       <c r="A34" s="58">
         <v>32</v>
       </c>
-      <c r="B34" s="59" t="str">
+      <c r="B34" s="92" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>4</v>
       </c>
@@ -6810,7 +6831,7 @@
       <c r="A35" s="47">
         <v>33</v>
       </c>
-      <c r="B35" s="48" t="str">
+      <c r="B35" s="93" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>5</v>
       </c>
@@ -6889,7 +6910,7 @@
       <c r="A36" s="56">
         <v>34</v>
       </c>
-      <c r="B36" s="43" t="str">
+      <c r="B36" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>5</v>
       </c>
@@ -6968,7 +6989,7 @@
       <c r="A37" s="56">
         <v>35</v>
       </c>
-      <c r="B37" s="43" t="str">
+      <c r="B37" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>5</v>
       </c>
@@ -7047,7 +7068,7 @@
       <c r="A38" s="56">
         <v>36</v>
       </c>
-      <c r="B38" s="43" t="str">
+      <c r="B38" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>5</v>
       </c>
@@ -7126,7 +7147,7 @@
       <c r="A39" s="56">
         <v>37</v>
       </c>
-      <c r="B39" s="43" t="str">
+      <c r="B39" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>5</v>
       </c>
@@ -7205,7 +7226,7 @@
       <c r="A40" s="56">
         <v>38</v>
       </c>
-      <c r="B40" s="43" t="str">
+      <c r="B40" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>5</v>
       </c>
@@ -7284,7 +7305,7 @@
       <c r="A41" s="56">
         <v>39</v>
       </c>
-      <c r="B41" s="43" t="str">
+      <c r="B41" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>5</v>
       </c>
@@ -7363,7 +7384,7 @@
       <c r="A42" s="58">
         <v>40</v>
       </c>
-      <c r="B42" s="59" t="str">
+      <c r="B42" s="92" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>5</v>
       </c>
@@ -7442,7 +7463,7 @@
       <c r="A43" s="47">
         <v>41</v>
       </c>
-      <c r="B43" s="48" t="str">
+      <c r="B43" s="93" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>6</v>
       </c>
@@ -7521,7 +7542,7 @@
       <c r="A44" s="56">
         <v>42</v>
       </c>
-      <c r="B44" s="43" t="str">
+      <c r="B44" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>6</v>
       </c>
@@ -7600,7 +7621,7 @@
       <c r="A45" s="56">
         <v>43</v>
       </c>
-      <c r="B45" s="43" t="str">
+      <c r="B45" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>6</v>
       </c>
@@ -7679,7 +7700,7 @@
       <c r="A46" s="56">
         <v>44</v>
       </c>
-      <c r="B46" s="43" t="str">
+      <c r="B46" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>6</v>
       </c>
@@ -7758,7 +7779,7 @@
       <c r="A47" s="56">
         <v>45</v>
       </c>
-      <c r="B47" s="43" t="str">
+      <c r="B47" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>6</v>
       </c>
@@ -7837,7 +7858,7 @@
       <c r="A48" s="56">
         <v>46</v>
       </c>
-      <c r="B48" s="43" t="str">
+      <c r="B48" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>6</v>
       </c>
@@ -7916,7 +7937,7 @@
       <c r="A49" s="56">
         <v>47</v>
       </c>
-      <c r="B49" s="43" t="str">
+      <c r="B49" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>6</v>
       </c>
@@ -7995,7 +8016,7 @@
       <c r="A50" s="58">
         <v>48</v>
       </c>
-      <c r="B50" s="59" t="str">
+      <c r="B50" s="92" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>6</v>
       </c>
@@ -8074,7 +8095,7 @@
       <c r="A51" s="47">
         <v>49</v>
       </c>
-      <c r="B51" s="48" t="str">
+      <c r="B51" s="93" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>7</v>
       </c>
@@ -8153,7 +8174,7 @@
       <c r="A52" s="56">
         <v>50</v>
       </c>
-      <c r="B52" s="43" t="str">
+      <c r="B52" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>7</v>
       </c>
@@ -8232,7 +8253,7 @@
       <c r="A53" s="56">
         <v>51</v>
       </c>
-      <c r="B53" s="43" t="str">
+      <c r="B53" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>7</v>
       </c>
@@ -8311,7 +8332,7 @@
       <c r="A54" s="56">
         <v>52</v>
       </c>
-      <c r="B54" s="43" t="str">
+      <c r="B54" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>7</v>
       </c>
@@ -8390,7 +8411,7 @@
       <c r="A55" s="56">
         <v>53</v>
       </c>
-      <c r="B55" s="43" t="str">
+      <c r="B55" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>7</v>
       </c>
@@ -8469,7 +8490,7 @@
       <c r="A56" s="56">
         <v>54</v>
       </c>
-      <c r="B56" s="43" t="str">
+      <c r="B56" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>7</v>
       </c>
@@ -8548,7 +8569,7 @@
       <c r="A57" s="56">
         <v>55</v>
       </c>
-      <c r="B57" s="43" t="str">
+      <c r="B57" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>7</v>
       </c>
@@ -8627,7 +8648,7 @@
       <c r="A58" s="58">
         <v>56</v>
       </c>
-      <c r="B58" s="59" t="str">
+      <c r="B58" s="92" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>7</v>
       </c>
@@ -8706,7 +8727,7 @@
       <c r="A59" s="47">
         <v>57</v>
       </c>
-      <c r="B59" s="48" t="str">
+      <c r="B59" s="93" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>8</v>
       </c>
@@ -8785,7 +8806,7 @@
       <c r="A60" s="56">
         <v>58</v>
       </c>
-      <c r="B60" s="43" t="str">
+      <c r="B60" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>8</v>
       </c>
@@ -8864,7 +8885,7 @@
       <c r="A61" s="56">
         <v>59</v>
       </c>
-      <c r="B61" s="43" t="str">
+      <c r="B61" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>8</v>
       </c>
@@ -8943,7 +8964,7 @@
       <c r="A62" s="56">
         <v>60</v>
       </c>
-      <c r="B62" s="43" t="str">
+      <c r="B62" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>8</v>
       </c>
@@ -9022,7 +9043,7 @@
       <c r="A63" s="56">
         <v>61</v>
       </c>
-      <c r="B63" s="43" t="str">
+      <c r="B63" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>8</v>
       </c>
@@ -9101,7 +9122,7 @@
       <c r="A64" s="56">
         <v>62</v>
       </c>
-      <c r="B64" s="43" t="str">
+      <c r="B64" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>8</v>
       </c>
@@ -9180,7 +9201,7 @@
       <c r="A65" s="56">
         <v>63</v>
       </c>
-      <c r="B65" s="43" t="str">
+      <c r="B65" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>8</v>
       </c>
@@ -9259,7 +9280,7 @@
       <c r="A66" s="58">
         <v>64</v>
       </c>
-      <c r="B66" s="59" t="str">
+      <c r="B66" s="92" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>8</v>
       </c>
@@ -9338,7 +9359,7 @@
       <c r="A67" s="47">
         <v>65</v>
       </c>
-      <c r="B67" s="48" t="str">
+      <c r="B67" s="93" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>9</v>
       </c>
@@ -9417,7 +9438,7 @@
       <c r="A68" s="56">
         <v>66</v>
       </c>
-      <c r="B68" s="43" t="str">
+      <c r="B68" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>9</v>
       </c>
@@ -9496,7 +9517,7 @@
       <c r="A69" s="56">
         <v>67</v>
       </c>
-      <c r="B69" s="43" t="str">
+      <c r="B69" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>9</v>
       </c>
@@ -9575,7 +9596,7 @@
       <c r="A70" s="56">
         <v>68</v>
       </c>
-      <c r="B70" s="43" t="str">
+      <c r="B70" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>9</v>
       </c>
@@ -9654,7 +9675,7 @@
       <c r="A71" s="56">
         <v>69</v>
       </c>
-      <c r="B71" s="43" t="str">
+      <c r="B71" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>9</v>
       </c>
@@ -9733,7 +9754,7 @@
       <c r="A72" s="56">
         <v>70</v>
       </c>
-      <c r="B72" s="43" t="str">
+      <c r="B72" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>9</v>
       </c>
@@ -9812,7 +9833,7 @@
       <c r="A73" s="56">
         <v>71</v>
       </c>
-      <c r="B73" s="43" t="str">
+      <c r="B73" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>9</v>
       </c>
@@ -9891,7 +9912,7 @@
       <c r="A74" s="58">
         <v>72</v>
       </c>
-      <c r="B74" s="59" t="str">
+      <c r="B74" s="92" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>9</v>
       </c>
@@ -9970,7 +9991,7 @@
       <c r="A75" s="47">
         <v>73</v>
       </c>
-      <c r="B75" s="48" t="str">
+      <c r="B75" s="93" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>10</v>
       </c>
@@ -10049,7 +10070,7 @@
       <c r="A76" s="56">
         <v>74</v>
       </c>
-      <c r="B76" s="43" t="str">
+      <c r="B76" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>10</v>
       </c>
@@ -10128,7 +10149,7 @@
       <c r="A77" s="56">
         <v>75</v>
       </c>
-      <c r="B77" s="43" t="str">
+      <c r="B77" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>10</v>
       </c>
@@ -10207,7 +10228,7 @@
       <c r="A78" s="56">
         <v>76</v>
       </c>
-      <c r="B78" s="43" t="str">
+      <c r="B78" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>10</v>
       </c>
@@ -10286,7 +10307,7 @@
       <c r="A79" s="56">
         <v>77</v>
       </c>
-      <c r="B79" s="43" t="str">
+      <c r="B79" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>10</v>
       </c>
@@ -10365,7 +10386,7 @@
       <c r="A80" s="56">
         <v>78</v>
       </c>
-      <c r="B80" s="43" t="str">
+      <c r="B80" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>10</v>
       </c>
@@ -10444,7 +10465,7 @@
       <c r="A81" s="56">
         <v>79</v>
       </c>
-      <c r="B81" s="43" t="str">
+      <c r="B81" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>10</v>
       </c>
@@ -10523,7 +10544,7 @@
       <c r="A82" s="58">
         <v>80</v>
       </c>
-      <c r="B82" s="59" t="str">
+      <c r="B82" s="92" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>10</v>
       </c>
@@ -10602,7 +10623,7 @@
       <c r="A83" s="47">
         <v>81</v>
       </c>
-      <c r="B83" s="48" t="str">
+      <c r="B83" s="93" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>11</v>
       </c>
@@ -10681,7 +10702,7 @@
       <c r="A84" s="56">
         <v>82</v>
       </c>
-      <c r="B84" s="43" t="str">
+      <c r="B84" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>11</v>
       </c>
@@ -10760,7 +10781,7 @@
       <c r="A85" s="56">
         <v>83</v>
       </c>
-      <c r="B85" s="43" t="str">
+      <c r="B85" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>11</v>
       </c>
@@ -10839,7 +10860,7 @@
       <c r="A86" s="56">
         <v>84</v>
       </c>
-      <c r="B86" s="43" t="str">
+      <c r="B86" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>11</v>
       </c>
@@ -10918,7 +10939,7 @@
       <c r="A87" s="56">
         <v>85</v>
       </c>
-      <c r="B87" s="43" t="str">
+      <c r="B87" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>11</v>
       </c>
@@ -10997,7 +11018,7 @@
       <c r="A88" s="56">
         <v>86</v>
       </c>
-      <c r="B88" s="43" t="str">
+      <c r="B88" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>11</v>
       </c>
@@ -11076,7 +11097,7 @@
       <c r="A89" s="56">
         <v>87</v>
       </c>
-      <c r="B89" s="43" t="str">
+      <c r="B89" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>11</v>
       </c>
@@ -11155,7 +11176,7 @@
       <c r="A90" s="58">
         <v>88</v>
       </c>
-      <c r="B90" s="59" t="str">
+      <c r="B90" s="92" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>11</v>
       </c>
@@ -11234,7 +11255,7 @@
       <c r="A91" s="47">
         <v>89</v>
       </c>
-      <c r="B91" s="48" t="str">
+      <c r="B91" s="93" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>12</v>
       </c>
@@ -11313,7 +11334,7 @@
       <c r="A92" s="56">
         <v>90</v>
       </c>
-      <c r="B92" s="43" t="str">
+      <c r="B92" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>12</v>
       </c>
@@ -11392,7 +11413,7 @@
       <c r="A93" s="56">
         <v>91</v>
       </c>
-      <c r="B93" s="43" t="str">
+      <c r="B93" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>12</v>
       </c>
@@ -11471,7 +11492,7 @@
       <c r="A94" s="56">
         <v>92</v>
       </c>
-      <c r="B94" s="43" t="str">
+      <c r="B94" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>12</v>
       </c>
@@ -11550,7 +11571,7 @@
       <c r="A95" s="56">
         <v>93</v>
       </c>
-      <c r="B95" s="43" t="str">
+      <c r="B95" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>12</v>
       </c>
@@ -11629,7 +11650,7 @@
       <c r="A96" s="56">
         <v>94</v>
       </c>
-      <c r="B96" s="43" t="str">
+      <c r="B96" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>12</v>
       </c>
@@ -11708,7 +11729,7 @@
       <c r="A97" s="56">
         <v>95</v>
       </c>
-      <c r="B97" s="43" t="str">
+      <c r="B97" s="91" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>12</v>
       </c>
@@ -11787,7 +11808,7 @@
       <c r="A98" s="58">
         <v>96</v>
       </c>
-      <c r="B98" s="59" t="str">
+      <c r="B98" s="92" t="str">
         <f>RIGHT(tbl_SeqLib[[#This Row],[Well]],LEN(tbl_SeqLib[[#This Row],[Well]])-1)</f>
         <v>12</v>
       </c>
@@ -11878,6 +11899,7 @@
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
       <c r="E100" s="2"/>
+      <c r="F100" s="2"/>
       <c r="G100" s="2"/>
       <c r="H100" s="2"/>
     </row>
@@ -11887,6 +11909,7 @@
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
+      <c r="F101" s="2"/>
       <c r="G101" s="2"/>
       <c r="H101" s="2"/>
     </row>
@@ -11896,6 +11919,7 @@
       <c r="C102" s="2"/>
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
+      <c r="F102" s="2"/>
       <c r="G102" s="2"/>
       <c r="H102" s="2"/>
     </row>
@@ -11905,6 +11929,7 @@
       <c r="C103" s="2"/>
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
+      <c r="F103" s="2"/>
       <c r="G103" s="2"/>
       <c r="H103" s="2"/>
     </row>
@@ -11914,6 +11939,7 @@
       <c r="C104" s="2"/>
       <c r="D104" s="2"/>
       <c r="E104" s="2"/>
+      <c r="F104" s="2"/>
       <c r="G104" s="2"/>
       <c r="H104" s="2"/>
     </row>
@@ -11923,6 +11949,7 @@
       <c r="C105" s="2"/>
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
+      <c r="F105" s="2"/>
       <c r="G105" s="2"/>
       <c r="H105" s="2"/>
     </row>
@@ -11932,6 +11959,7 @@
       <c r="C106" s="2"/>
       <c r="D106" s="2"/>
       <c r="E106" s="2"/>
+      <c r="F106" s="2"/>
       <c r="G106" s="2"/>
       <c r="H106" s="2"/>
     </row>
@@ -11941,6 +11969,7 @@
       <c r="C107" s="2"/>
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
+      <c r="F107" s="2"/>
       <c r="G107" s="2"/>
       <c r="H107" s="2"/>
     </row>
@@ -11950,6 +11979,7 @@
       <c r="C108" s="2"/>
       <c r="D108" s="2"/>
       <c r="E108" s="2"/>
+      <c r="F108" s="2"/>
       <c r="G108" s="2"/>
       <c r="H108" s="2"/>
     </row>
@@ -11959,6 +11989,7 @@
       <c r="C109" s="2"/>
       <c r="D109" s="2"/>
       <c r="E109" s="2"/>
+      <c r="F109" s="2"/>
       <c r="G109" s="2"/>
       <c r="H109" s="2"/>
     </row>
@@ -11968,6 +11999,7 @@
       <c r="C110" s="2"/>
       <c r="D110" s="2"/>
       <c r="E110" s="2"/>
+      <c r="F110" s="2"/>
       <c r="G110" s="2"/>
       <c r="H110" s="2"/>
     </row>
@@ -11977,6 +12009,7 @@
       <c r="C111" s="2"/>
       <c r="D111" s="2"/>
       <c r="E111" s="2"/>
+      <c r="F111" s="2"/>
       <c r="G111" s="2"/>
       <c r="H111" s="2"/>
     </row>
@@ -11994,7 +12027,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="textLength" errorStyle="warning" operator="greaterThan" allowBlank="1" showErrorMessage="1" error="The Extraction ID cannot be left blank." prompt="Enter the Extraction ID" sqref="E10:E98 D3:E98 F4:F98" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="textLength" errorStyle="warning" operator="greaterThan" allowBlank="1" showErrorMessage="1" error="The Extraction ID cannot be left blank." prompt="Enter the Extraction ID" sqref="F4:F98 D3:F98" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -12272,7 +12305,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="E15" s="10" t="s">
         <v>329</v>
@@ -12386,22 +12419,22 @@
     </row>
     <row r="36" spans="5:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E36" s="86" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="37" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E37" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="38" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E38" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="39" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E39" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
   </sheetData>
@@ -12428,7 +12461,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -12809,9 +12842,9 @@
         <f>IF(LEN(exp_summary)=0,"",exp_summary)</f>
         <v/>
       </c>
-      <c r="I2" t="str">
+      <c r="I2">
         <f>IF(LEN(exp_rxns)=0,"",exp_rxns)</f>
-        <v/>
+        <v>10</v>
       </c>
       <c r="J2">
         <v>200</v>
@@ -12900,7 +12933,7 @@
         <v>303</v>
       </c>
       <c r="C1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="D1" t="s">
         <v>284</v>

</xml_diff>

<commit_message>
Minor corrections to template
</commit_message>
<xml_diff>
--- a/templates/NOMADS_Library_Rapid_Worksheet.xlsx
+++ b/templates/NOMADS_Library_Rapid_Worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\warehouse\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB5B4B05-1243-4E9E-9D50-4E25570CDEE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6C3256-B87E-4235-9607-ADBF7A45A060}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="34080" windowHeight="22200" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2444,58 +2444,46 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2516,32 +2504,41 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -2554,6 +2551,9 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -3427,8 +3427,8 @@
   </sheetPr>
   <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView topLeftCell="A14" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41:D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3437,171 +3437,171 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="96" t="s">
         <v>371</v>
       </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
-      <c r="D1" s="119"/>
-      <c r="E1" s="119"/>
-      <c r="F1" s="119"/>
-      <c r="G1" s="119"/>
-      <c r="H1" s="119"/>
-      <c r="I1" s="119"/>
-      <c r="J1" s="119"/>
-      <c r="K1" s="119"/>
-      <c r="L1" s="119"/>
+      <c r="B1" s="96"/>
+      <c r="C1" s="96"/>
+      <c r="D1" s="96"/>
+      <c r="E1" s="96"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="96"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="97" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="94"/>
-      <c r="C2" s="120"/>
-      <c r="D2" s="120"/>
-      <c r="E2" s="120"/>
-      <c r="F2" s="120"/>
-      <c r="G2" s="101" t="s">
+      <c r="B2" s="97"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="99" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="101"/>
-      <c r="J2" s="121" t="s">
+      <c r="H2" s="99"/>
+      <c r="J2" s="100" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="121"/>
+      <c r="K2" s="100"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="94" t="s">
+      <c r="A3" s="97" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="94"/>
-      <c r="C3" s="122"/>
-      <c r="D3" s="122"/>
-      <c r="E3" s="122"/>
-      <c r="F3" s="122"/>
+      <c r="B3" s="97"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="101"/>
+      <c r="F3" s="101"/>
       <c r="G3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="123" t="s">
+      <c r="J3" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="123"/>
+      <c r="K3" s="102"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="94" t="s">
+      <c r="A4" s="97" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="94"/>
-      <c r="C4" s="120"/>
-      <c r="D4" s="120"/>
-      <c r="E4" s="120"/>
-      <c r="F4" s="120"/>
+      <c r="B4" s="97"/>
+      <c r="C4" s="98"/>
+      <c r="D4" s="98"/>
+      <c r="E4" s="98"/>
+      <c r="F4" s="98"/>
       <c r="G4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="124" t="s">
+      <c r="J4" s="103" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="124"/>
+      <c r="K4" s="103"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="110" t="s">
+      <c r="A5" s="104" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="110"/>
-      <c r="C5" s="108" t="str">
+      <c r="B5" s="104"/>
+      <c r="C5" s="105" t="str">
         <f>IF(OR(ISBLANK(C3),ISBLANK(C4)),"",CONCATENATE("SL",VLOOKUP(C3,reference!H3:I9,2,FALSE()),C4))</f>
         <v/>
       </c>
-      <c r="D5" s="108"/>
-      <c r="E5" s="108"/>
-      <c r="F5" s="108"/>
+      <c r="D5" s="105"/>
+      <c r="E5" s="105"/>
+      <c r="F5" s="105"/>
       <c r="G5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="109" t="s">
+      <c r="J5" s="106" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="109"/>
+      <c r="K5" s="106"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="110" t="s">
+      <c r="A6" s="104" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="110"/>
-      <c r="C6" s="111" t="str">
+      <c r="B6" s="104"/>
+      <c r="C6" s="107" t="str">
         <f>IF(OR(ISBLANK(C2),ISBLANK(C3),ISBLANK(C4)),"",CONCATENATE(C2,"_SeqLib_",C5))</f>
         <v/>
       </c>
-      <c r="D6" s="111"/>
-      <c r="E6" s="111"/>
-      <c r="F6" s="111"/>
+      <c r="D6" s="107"/>
+      <c r="E6" s="107"/>
+      <c r="F6" s="107"/>
       <c r="G6" s="4"/>
-      <c r="J6" s="109"/>
-      <c r="K6" s="109"/>
+      <c r="J6" s="106"/>
+      <c r="K6" s="106"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="117" t="s">
+      <c r="A7" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="117"/>
-      <c r="C7" s="118"/>
-      <c r="D7" s="118"/>
-      <c r="E7" s="118"/>
-      <c r="F7" s="118"/>
+      <c r="B7" s="94"/>
+      <c r="C7" s="95"/>
+      <c r="D7" s="95"/>
+      <c r="E7" s="95"/>
+      <c r="F7" s="95"/>
       <c r="G7" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="117" t="s">
+      <c r="A8" s="94" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="117"/>
-      <c r="C8" s="118"/>
-      <c r="D8" s="118"/>
-      <c r="E8" s="118"/>
-      <c r="F8" s="118"/>
+      <c r="B8" s="94"/>
+      <c r="C8" s="95"/>
+      <c r="D8" s="95"/>
+      <c r="E8" s="95"/>
+      <c r="F8" s="95"/>
       <c r="G8" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="113" t="s">
+      <c r="A9" s="109" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="113"/>
-      <c r="C9" s="114" t="str">
+      <c r="B9" s="109"/>
+      <c r="C9" s="110" t="str">
         <f>IF(OR(LEN(C7)=0, LEN(C8)=0),"",CONCATENATE(C7,"_Batch",C8))</f>
         <v/>
       </c>
-      <c r="D9" s="114"/>
-      <c r="E9" s="114"/>
-      <c r="F9" s="114"/>
+      <c r="D9" s="110"/>
+      <c r="E9" s="110"/>
+      <c r="F9" s="110"/>
       <c r="G9" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="113" t="s">
+      <c r="A10" s="109" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="113"/>
-      <c r="C10" s="114" t="str">
+      <c r="B10" s="109"/>
+      <c r="C10" s="110" t="str">
         <f>IF(OR(LEN(C6)=0,LEN(exp_summary)=0),"",CONCATENATE(C6,"_",exp_summary))</f>
         <v/>
       </c>
-      <c r="D10" s="114"/>
-      <c r="E10" s="114"/>
-      <c r="F10" s="114"/>
-      <c r="G10" s="114"/>
-      <c r="H10" s="114"/>
+      <c r="D10" s="110"/>
+      <c r="E10" s="110"/>
+      <c r="F10" s="110"/>
+      <c r="G10" s="110"/>
+      <c r="H10" s="110"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="94" t="s">
+      <c r="A11" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="94"/>
+      <c r="B11" s="97"/>
       <c r="C11" s="26">
         <v>10</v>
       </c>
@@ -3611,32 +3611,32 @@
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="94" t="s">
+      <c r="A12" s="97" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="94"/>
-      <c r="C12" s="115"/>
-      <c r="D12" s="115"/>
-      <c r="E12" s="115"/>
-      <c r="F12" s="115"/>
-      <c r="G12" s="115"/>
-      <c r="H12" s="115"/>
-      <c r="I12" s="115"/>
-      <c r="J12" s="115"/>
-      <c r="K12" s="115"/>
+      <c r="B12" s="97"/>
+      <c r="C12" s="111"/>
+      <c r="D12" s="111"/>
+      <c r="E12" s="111"/>
+      <c r="F12" s="111"/>
+      <c r="G12" s="111"/>
+      <c r="H12" s="111"/>
+      <c r="I12" s="111"/>
+      <c r="J12" s="111"/>
+      <c r="K12" s="111"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="115"/>
-      <c r="D13" s="115"/>
-      <c r="E13" s="115"/>
-      <c r="F13" s="115"/>
-      <c r="G13" s="115"/>
-      <c r="H13" s="115"/>
-      <c r="I13" s="115"/>
-      <c r="J13" s="115"/>
-      <c r="K13" s="115"/>
+      <c r="C13" s="111"/>
+      <c r="D13" s="111"/>
+      <c r="E13" s="111"/>
+      <c r="F13" s="111"/>
+      <c r="G13" s="111"/>
+      <c r="H13" s="111"/>
+      <c r="I13" s="111"/>
+      <c r="J13" s="111"/>
+      <c r="K13" s="111"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C14" s="5"/>
@@ -3659,11 +3659,11 @@
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="H16" s="4"/>
-      <c r="I16" s="116" t="s">
+      <c r="I16" s="112" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="116"/>
-      <c r="K16" s="116"/>
+      <c r="J16" s="112"/>
+      <c r="K16" s="112"/>
     </row>
     <row r="17" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
@@ -3674,10 +3674,10 @@
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="G17" s="8"/>
-      <c r="I17" s="98" t="s">
+      <c r="I17" s="113" t="s">
         <v>25</v>
       </c>
-      <c r="J17" s="98"/>
+      <c r="J17" s="113"/>
       <c r="K17" s="9" t="s">
         <v>26</v>
       </c>
@@ -3689,10 +3689,10 @@
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="G18" s="8"/>
-      <c r="I18" s="112">
+      <c r="I18" s="108">
         <v>30</v>
       </c>
-      <c r="J18" s="112"/>
+      <c r="J18" s="108"/>
       <c r="K18" s="2" t="s">
         <v>27</v>
       </c>
@@ -3704,10 +3704,10 @@
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="G19" s="8"/>
-      <c r="I19" s="112">
+      <c r="I19" s="108">
         <v>30</v>
       </c>
-      <c r="J19" s="112"/>
+      <c r="J19" s="108"/>
       <c r="K19" s="7">
         <v>2</v>
       </c>
@@ -3719,10 +3719,10 @@
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="G20" s="8"/>
-      <c r="I20" s="112">
+      <c r="I20" s="108">
         <v>80</v>
       </c>
-      <c r="J20" s="112"/>
+      <c r="J20" s="108"/>
       <c r="K20" s="2">
         <v>2</v>
       </c>
@@ -3734,10 +3734,10 @@
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="G21" s="8"/>
-      <c r="I21" s="112">
+      <c r="I21" s="108">
         <v>8</v>
       </c>
-      <c r="J21" s="112"/>
+      <c r="J21" s="108"/>
       <c r="K21" s="2" t="s">
         <v>27</v>
       </c>
@@ -3760,21 +3760,21 @@
       <c r="G23" s="25"/>
     </row>
     <row r="24" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="101" t="str">
+      <c r="A24" s="99" t="str">
         <f>_xlfn.CONCAT("2. Clean up: Add 0.5x vol (", SUM(5*exp_rxns)*0.5,"µl) AMPPure beads for 5 min RT with mixing, wash with fresh 80% EtOH, spin, dry, re-suspend in 15 µl EB (10 min @RT) and transfer eluate to fresh tube")</f>
         <v>2. Clean up: Add 0.5x vol (25µl) AMPPure beads for 5 min RT with mixing, wash with fresh 80% EtOH, spin, dry, re-suspend in 15 µl EB (10 min @RT) and transfer eluate to fresh tube</v>
       </c>
-      <c r="B24" s="101"/>
-      <c r="C24" s="101"/>
-      <c r="D24" s="101"/>
-      <c r="E24" s="101"/>
-      <c r="F24" s="101"/>
-      <c r="G24" s="101"/>
-      <c r="H24" s="101"/>
-      <c r="I24" s="101"/>
-      <c r="J24" s="101"/>
-      <c r="K24" s="101"/>
-      <c r="L24" s="101"/>
+      <c r="B24" s="99"/>
+      <c r="C24" s="99"/>
+      <c r="D24" s="99"/>
+      <c r="E24" s="99"/>
+      <c r="F24" s="99"/>
+      <c r="G24" s="99"/>
+      <c r="H24" s="99"/>
+      <c r="I24" s="99"/>
+      <c r="J24" s="99"/>
+      <c r="K24" s="99"/>
+      <c r="L24" s="99"/>
     </row>
     <row r="25" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
@@ -3797,18 +3797,18 @@
       <c r="C26" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="102" t="s">
+      <c r="D26" s="116" t="s">
         <v>32</v>
       </c>
-      <c r="E26" s="102"/>
-      <c r="F26" s="105" t="s">
+      <c r="E26" s="116"/>
+      <c r="F26" s="118" t="s">
         <v>388</v>
       </c>
-      <c r="G26" s="105"/>
-      <c r="H26" s="105" t="s">
+      <c r="G26" s="118"/>
+      <c r="H26" s="118" t="s">
         <v>392</v>
       </c>
-      <c r="I26" s="105"/>
+      <c r="I26" s="118"/>
     </row>
     <row r="27" spans="1:17" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
@@ -3819,21 +3819,21 @@
       <c r="C27" s="31">
         <v>10</v>
       </c>
-      <c r="D27" s="103">
+      <c r="D27" s="117">
         <f>SUM(B27*C27)</f>
         <v>0</v>
       </c>
-      <c r="E27" s="103"/>
-      <c r="F27" s="104" t="str">
+      <c r="E27" s="117"/>
+      <c r="F27" s="127" t="str">
         <f>IFERROR(IF(SUM(flowcell_targetmass/DNAconc_pooled)&gt;flowcell_maxvol-1,flowcell_maxvol-1, SUM(flowcell_targetmass/DNAconc_pooled)),"")</f>
         <v/>
       </c>
-      <c r="G27" s="104"/>
-      <c r="H27" s="104" t="str">
+      <c r="G27" s="127"/>
+      <c r="H27" s="127" t="str">
         <f>IFERROR(SUM(10-F27),"")</f>
         <v/>
       </c>
-      <c r="I27" s="104"/>
+      <c r="I27" s="127"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
@@ -3870,48 +3870,48 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="98" t="s">
+      <c r="A35" s="113" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="98"/>
-      <c r="C35" s="98"/>
-      <c r="D35" s="106" t="s">
+      <c r="B35" s="113"/>
+      <c r="C35" s="113"/>
+      <c r="D35" s="119" t="s">
         <v>24</v>
       </c>
-      <c r="E35" s="106"/>
+      <c r="E35" s="119"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="102" t="s">
+      <c r="A36" s="116" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="102"/>
-      <c r="C36" s="102"/>
-      <c r="D36" s="107">
+      <c r="B36" s="116"/>
+      <c r="C36" s="116"/>
+      <c r="D36" s="120">
         <v>11</v>
       </c>
-      <c r="E36" s="107"/>
+      <c r="E36" s="120"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="99" t="s">
+      <c r="A37" s="114" t="s">
         <v>394</v>
       </c>
-      <c r="B37" s="99"/>
-      <c r="C37" s="99"/>
-      <c r="D37" s="100">
+      <c r="B37" s="114"/>
+      <c r="C37" s="114"/>
+      <c r="D37" s="115">
         <v>37.5</v>
       </c>
-      <c r="E37" s="100"/>
+      <c r="E37" s="115"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="99" t="s">
+      <c r="A38" s="114" t="s">
         <v>395</v>
       </c>
-      <c r="B38" s="99"/>
-      <c r="C38" s="99"/>
-      <c r="D38" s="100">
+      <c r="B38" s="114"/>
+      <c r="C38" s="114"/>
+      <c r="D38" s="115">
         <v>25.5</v>
       </c>
-      <c r="E38" s="100"/>
+      <c r="E38" s="115"/>
       <c r="F38" s="4" t="s">
         <v>35</v>
       </c>
@@ -3923,75 +3923,75 @@
       <c r="C40" s="4"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="94" t="s">
+      <c r="A41" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="B41" s="94"/>
-      <c r="C41" s="96"/>
-      <c r="D41" s="96"/>
+      <c r="B41" s="97"/>
+      <c r="C41" s="122"/>
+      <c r="D41" s="122"/>
       <c r="E41" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="94" t="s">
+      <c r="A42" s="97" t="s">
         <v>39</v>
       </c>
-      <c r="B42" s="94"/>
-      <c r="C42" s="95"/>
-      <c r="D42" s="95"/>
+      <c r="B42" s="97"/>
+      <c r="C42" s="121"/>
+      <c r="D42" s="121"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="94" t="s">
+      <c r="A43" s="97" t="s">
         <v>40</v>
       </c>
-      <c r="B43" s="94"/>
-      <c r="C43" s="95"/>
-      <c r="D43" s="95"/>
+      <c r="B43" s="97"/>
+      <c r="C43" s="121"/>
+      <c r="D43" s="121"/>
     </row>
     <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="94" t="s">
+      <c r="A44" s="97" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="94"/>
-      <c r="C44" s="97" t="str">
+      <c r="B44" s="97"/>
+      <c r="C44" s="123" t="str">
         <f>IF(flowcell_status="New",0,"")</f>
         <v/>
       </c>
-      <c r="D44" s="97"/>
+      <c r="D44" s="123"/>
       <c r="E44" s="8" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="94" t="s">
+      <c r="A45" s="97" t="s">
         <v>43</v>
       </c>
-      <c r="B45" s="94"/>
-      <c r="C45" s="96"/>
-      <c r="D45" s="96"/>
+      <c r="B45" s="97"/>
+      <c r="C45" s="122"/>
+      <c r="D45" s="122"/>
       <c r="E45" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="94" t="s">
+      <c r="A46" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="94"/>
-      <c r="C46" s="95"/>
-      <c r="D46" s="95"/>
+      <c r="B46" s="97"/>
+      <c r="C46" s="121"/>
+      <c r="D46" s="121"/>
       <c r="E46" s="8" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="94" t="s">
+      <c r="A47" s="97" t="s">
         <v>47</v>
       </c>
-      <c r="B47" s="94"/>
-      <c r="C47" s="95"/>
-      <c r="D47" s="95"/>
+      <c r="B47" s="97"/>
+      <c r="C47" s="121"/>
+      <c r="D47" s="121"/>
       <c r="E47" s="8" t="s">
         <v>48</v>
       </c>
@@ -3999,6 +3999,52 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="62">
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="C47:D47"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A24:L24"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="J5:K6"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="C10:H10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:K13"/>
+    <mergeCell ref="I16:K16"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="C7:F7"/>
     <mergeCell ref="A8:B8"/>
@@ -4015,52 +4061,6 @@
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="J5:K6"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="I21:J21"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="C10:H10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="C12:K13"/>
-    <mergeCell ref="I16:K16"/>
-    <mergeCell ref="I17:J17"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A24:L24"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="C45:D45"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:C4 C7:C8 C11:C12 B27:C27 C41:C43 C45:C47">
     <cfRule type="expression" dxfId="6" priority="7">
@@ -4187,37 +4187,37 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C1" s="44"/>
-      <c r="D1" s="125" t="s">
+      <c r="D1" s="124" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="125"/>
-      <c r="F1" s="125"/>
+      <c r="E1" s="124"/>
+      <c r="F1" s="124"/>
       <c r="G1" s="68" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="126" t="s">
+      <c r="H1" s="125" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="126"/>
-      <c r="J1" s="126"/>
-      <c r="K1" s="126"/>
-      <c r="L1" s="127" t="s">
+      <c r="I1" s="125"/>
+      <c r="J1" s="125"/>
+      <c r="K1" s="125"/>
+      <c r="L1" s="126" t="s">
         <v>52</v>
       </c>
-      <c r="M1" s="127"/>
-      <c r="N1" s="127"/>
-      <c r="O1" s="127"/>
-      <c r="P1" s="127"/>
-      <c r="Q1" s="127"/>
-      <c r="R1" s="127"/>
-      <c r="S1" s="127"/>
-      <c r="T1" s="127"/>
-      <c r="U1" s="127"/>
-      <c r="V1" s="127"/>
-      <c r="W1" s="127"/>
-      <c r="X1" s="127"/>
-      <c r="Y1" s="127"/>
-      <c r="Z1" s="127"/>
+      <c r="M1" s="126"/>
+      <c r="N1" s="126"/>
+      <c r="O1" s="126"/>
+      <c r="P1" s="126"/>
+      <c r="Q1" s="126"/>
+      <c r="R1" s="126"/>
+      <c r="S1" s="126"/>
+      <c r="T1" s="126"/>
+      <c r="U1" s="126"/>
+      <c r="V1" s="126"/>
+      <c r="W1" s="126"/>
+      <c r="X1" s="126"/>
+      <c r="Y1" s="126"/>
+      <c r="Z1" s="126"/>
     </row>
     <row r="2" spans="1:26" s="10" customFormat="1" ht="81" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="46" t="s">
@@ -12461,7 +12461,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Corrected dropdown definitions for warehouse template
</commit_message>
<xml_diff>
--- a/templates/NOMADS_Library_Rapid_Worksheet.xlsx
+++ b/templates/NOMADS_Library_Rapid_Worksheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\warehouse\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DC38A2C-1D36-495F-A5EF-E14F393BAD28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA453963-14E5-4A4D-9336-3B264A16102B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="34080" windowHeight="22200" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="29100" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assay" sheetId="1" r:id="rId1"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="405">
   <si>
     <t>Date:</t>
   </si>
@@ -1285,9 +1285,6 @@
   </si>
   <si>
     <t>Flow Chemistry</t>
-  </si>
-  <si>
-    <t>R9.4.1</t>
   </si>
   <si>
     <t>Column</t>
@@ -2494,8 +2491,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -2504,6 +2502,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -2573,10 +2574,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2590,14 +2587,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC00000"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3457,7 +3454,7 @@
   <dimension ref="A1:Q47"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="C47" sqref="C47:D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3466,174 +3463,172 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="120" t="s">
-        <v>368</v>
-      </c>
-      <c r="B1" s="120"/>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="120"/>
-      <c r="G1" s="120"/>
-      <c r="H1" s="120"/>
-      <c r="I1" s="120"/>
-      <c r="J1" s="120"/>
-      <c r="K1" s="120"/>
-      <c r="L1" s="120"/>
+      <c r="A1" s="121" t="s">
+        <v>367</v>
+      </c>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
+      <c r="D1" s="121"/>
+      <c r="E1" s="121"/>
+      <c r="F1" s="121"/>
+      <c r="G1" s="121"/>
+      <c r="H1" s="121"/>
+      <c r="I1" s="121"/>
+      <c r="J1" s="121"/>
+      <c r="K1" s="121"/>
+      <c r="L1" s="121"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="95" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="95"/>
-      <c r="C2" s="121"/>
-      <c r="D2" s="121"/>
-      <c r="E2" s="121"/>
-      <c r="F2" s="121"/>
+      <c r="C2" s="122"/>
+      <c r="D2" s="122"/>
+      <c r="E2" s="122"/>
+      <c r="F2" s="122"/>
       <c r="G2" s="102" t="s">
         <v>1</v>
       </c>
       <c r="H2" s="102"/>
-      <c r="J2" s="122" t="s">
+      <c r="J2" s="123" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="122"/>
+      <c r="K2" s="123"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="95" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="95"/>
-      <c r="C3" s="123"/>
-      <c r="D3" s="123"/>
-      <c r="E3" s="123"/>
-      <c r="F3" s="123"/>
+      <c r="C3" s="124"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="124"/>
+      <c r="F3" s="124"/>
       <c r="G3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="124" t="s">
+      <c r="J3" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="124"/>
+      <c r="K3" s="125"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="95" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="95"/>
-      <c r="C4" s="121"/>
-      <c r="D4" s="121"/>
-      <c r="E4" s="121"/>
-      <c r="F4" s="121"/>
+      <c r="C4" s="122"/>
+      <c r="D4" s="122"/>
+      <c r="E4" s="122"/>
+      <c r="F4" s="122"/>
       <c r="G4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="125" t="s">
+      <c r="J4" s="126" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="125"/>
+      <c r="K4" s="126"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="111" t="s">
+      <c r="A5" s="112" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="111"/>
-      <c r="C5" s="109" t="str">
+      <c r="B5" s="112"/>
+      <c r="C5" s="110" t="str">
         <f>IF(OR(ISBLANK(C3),ISBLANK(C4)),"",CONCATENATE("SL",VLOOKUP(C3,reference!I3:J9,2,FALSE()),C4))</f>
         <v/>
       </c>
-      <c r="D5" s="109"/>
-      <c r="E5" s="109"/>
-      <c r="F5" s="109"/>
+      <c r="D5" s="110"/>
+      <c r="E5" s="110"/>
+      <c r="F5" s="110"/>
       <c r="G5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="110" t="s">
+      <c r="J5" s="111" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="110"/>
+      <c r="K5" s="111"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="111" t="s">
+      <c r="A6" s="112" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="111"/>
-      <c r="C6" s="112" t="str">
+      <c r="B6" s="112"/>
+      <c r="C6" s="113" t="str">
         <f>IF(OR(ISBLANK(C2),ISBLANK(C3),ISBLANK(C4)),"",CONCATENATE(C2,"_SeqLib_",C5))</f>
         <v/>
       </c>
-      <c r="D6" s="112"/>
-      <c r="E6" s="112"/>
-      <c r="F6" s="112"/>
+      <c r="D6" s="113"/>
+      <c r="E6" s="113"/>
+      <c r="F6" s="113"/>
       <c r="G6" s="4"/>
-      <c r="J6" s="110"/>
-      <c r="K6" s="110"/>
+      <c r="J6" s="111"/>
+      <c r="K6" s="111"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="118" t="s">
+      <c r="A7" s="119" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="118"/>
-      <c r="C7" s="119"/>
-      <c r="D7" s="119"/>
-      <c r="E7" s="119"/>
-      <c r="F7" s="119"/>
+      <c r="B7" s="119"/>
+      <c r="C7" s="120"/>
+      <c r="D7" s="120"/>
+      <c r="E7" s="120"/>
+      <c r="F7" s="120"/>
       <c r="G7" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="118" t="s">
+      <c r="A8" s="119" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="118"/>
-      <c r="C8" s="119"/>
-      <c r="D8" s="119"/>
-      <c r="E8" s="119"/>
-      <c r="F8" s="119"/>
+      <c r="B8" s="119"/>
+      <c r="C8" s="120"/>
+      <c r="D8" s="120"/>
+      <c r="E8" s="120"/>
+      <c r="F8" s="120"/>
       <c r="G8" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="114" t="s">
+      <c r="A9" s="115" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="114"/>
-      <c r="C9" s="115" t="str">
+      <c r="B9" s="115"/>
+      <c r="C9" s="116" t="str">
         <f>IF(OR(LEN(C7)=0, LEN(C8)=0),"",CONCATENATE(C7,"_Batch",C8))</f>
         <v/>
       </c>
-      <c r="D9" s="115"/>
-      <c r="E9" s="115"/>
-      <c r="F9" s="115"/>
+      <c r="D9" s="116"/>
+      <c r="E9" s="116"/>
+      <c r="F9" s="116"/>
       <c r="G9" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="114" t="s">
+      <c r="A10" s="115" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="114"/>
-      <c r="C10" s="115" t="str">
+      <c r="B10" s="115"/>
+      <c r="C10" s="116" t="str">
         <f>IF(OR(LEN(C6)=0,LEN(exp_summary)=0),"",CONCATENATE(C6,"_",exp_summary))</f>
         <v/>
       </c>
-      <c r="D10" s="115"/>
-      <c r="E10" s="115"/>
-      <c r="F10" s="115"/>
-      <c r="G10" s="115"/>
-      <c r="H10" s="115"/>
+      <c r="D10" s="116"/>
+      <c r="E10" s="116"/>
+      <c r="F10" s="116"/>
+      <c r="G10" s="116"/>
+      <c r="H10" s="116"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="95" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="95"/>
-      <c r="C11" s="26">
-        <v>10</v>
-      </c>
+      <c r="C11" s="26"/>
       <c r="D11" s="24"/>
       <c r="E11" s="24"/>
       <c r="F11" s="24"/>
@@ -3644,28 +3639,28 @@
         <v>20</v>
       </c>
       <c r="B12" s="95"/>
-      <c r="C12" s="116"/>
-      <c r="D12" s="116"/>
-      <c r="E12" s="116"/>
-      <c r="F12" s="116"/>
-      <c r="G12" s="116"/>
-      <c r="H12" s="116"/>
-      <c r="I12" s="116"/>
-      <c r="J12" s="116"/>
-      <c r="K12" s="116"/>
+      <c r="C12" s="117"/>
+      <c r="D12" s="117"/>
+      <c r="E12" s="117"/>
+      <c r="F12" s="117"/>
+      <c r="G12" s="117"/>
+      <c r="H12" s="117"/>
+      <c r="I12" s="117"/>
+      <c r="J12" s="117"/>
+      <c r="K12" s="117"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="116"/>
-      <c r="D13" s="116"/>
-      <c r="E13" s="116"/>
-      <c r="F13" s="116"/>
-      <c r="G13" s="116"/>
-      <c r="H13" s="116"/>
-      <c r="I13" s="116"/>
-      <c r="J13" s="116"/>
-      <c r="K13" s="116"/>
+      <c r="C13" s="117"/>
+      <c r="D13" s="117"/>
+      <c r="E13" s="117"/>
+      <c r="F13" s="117"/>
+      <c r="G13" s="117"/>
+      <c r="H13" s="117"/>
+      <c r="I13" s="117"/>
+      <c r="J13" s="117"/>
+      <c r="K13" s="117"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C14" s="5"/>
@@ -3688,15 +3683,15 @@
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="H16" s="4"/>
-      <c r="I16" s="117" t="s">
+      <c r="I16" s="118" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="117"/>
-      <c r="K16" s="117"/>
+      <c r="J16" s="118"/>
+      <c r="K16" s="118"/>
     </row>
     <row r="17" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -3718,10 +3713,10 @@
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="G18" s="8"/>
-      <c r="I18" s="113">
+      <c r="I18" s="114">
         <v>30</v>
       </c>
-      <c r="J18" s="113"/>
+      <c r="J18" s="114"/>
       <c r="K18" s="2" t="s">
         <v>27</v>
       </c>
@@ -3733,10 +3728,10 @@
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="G19" s="8"/>
-      <c r="I19" s="113">
+      <c r="I19" s="114">
         <v>30</v>
       </c>
-      <c r="J19" s="113"/>
+      <c r="J19" s="114"/>
       <c r="K19" s="7">
         <v>2</v>
       </c>
@@ -3748,10 +3743,10 @@
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="G20" s="8"/>
-      <c r="I20" s="113">
+      <c r="I20" s="114">
         <v>80</v>
       </c>
-      <c r="J20" s="113"/>
+      <c r="J20" s="114"/>
       <c r="K20" s="2">
         <v>2</v>
       </c>
@@ -3763,10 +3758,10 @@
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="G21" s="8"/>
-      <c r="I21" s="113">
+      <c r="I21" s="114">
         <v>8</v>
       </c>
-      <c r="J21" s="113"/>
+      <c r="J21" s="114"/>
       <c r="K21" s="2" t="s">
         <v>27</v>
       </c>
@@ -3779,7 +3774,7 @@
     </row>
     <row r="23" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -3791,7 +3786,7 @@
     <row r="24" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="102" t="str">
         <f>_xlfn.CONCAT("2. Clean up: Add 0.5x vol (", SUM(5*exp_rxns)*0.5,"µl) AMPPure beads for 5 min RT with mixing, wash with fresh 80% EtOH, spin, dry, re-suspend in 15 µl EB (10 min @RT) and transfer eluate to fresh tube")</f>
-        <v>2. Clean up: Add 0.5x vol (25µl) AMPPure beads for 5 min RT with mixing, wash with fresh 80% EtOH, spin, dry, re-suspend in 15 µl EB (10 min @RT) and transfer eluate to fresh tube</v>
+        <v>2. Clean up: Add 0.5x vol (0µl) AMPPure beads for 5 min RT with mixing, wash with fresh 80% EtOH, spin, dry, re-suspend in 15 µl EB (10 min @RT) and transfer eluate to fresh tube</v>
       </c>
       <c r="B24" s="102"/>
       <c r="C24" s="102"/>
@@ -3807,7 +3802,7 @@
     </row>
     <row r="25" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -3831,18 +3826,18 @@
       </c>
       <c r="E26" s="103"/>
       <c r="F26" s="106" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="G26" s="106"/>
       <c r="H26" s="106" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I26" s="106"/>
     </row>
     <row r="27" spans="1:17" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
         <f>SUM(exp_rxns*5)*0.5</f>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="B27" s="31"/>
       <c r="C27" s="31">
@@ -3853,16 +3848,16 @@
         <v>0</v>
       </c>
       <c r="E27" s="104"/>
-      <c r="F27" s="129" t="str">
+      <c r="F27" s="105" t="str">
         <f>IFERROR(IF(SUM(flowcell_targetmass/DNAconc_pooled)&gt;flowcell_maxvol-1,flowcell_maxvol-1, SUM(flowcell_targetmass/DNAconc_pooled)),"")</f>
         <v/>
       </c>
-      <c r="G27" s="129"/>
-      <c r="H27" s="105" t="str">
+      <c r="G27" s="105"/>
+      <c r="H27" s="109" t="str">
         <f>IFERROR(SUM(11-F27),"")</f>
         <v/>
       </c>
-      <c r="I27" s="105"/>
+      <c r="I27" s="109"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
@@ -3871,7 +3866,7 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -3879,14 +3874,14 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
@@ -3895,7 +3890,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3922,7 +3917,7 @@
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="100" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B37" s="100"/>
       <c r="C37" s="100"/>
@@ -3933,7 +3928,7 @@
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="100" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B38" s="100"/>
       <c r="C38" s="100"/>
@@ -3997,7 +3992,9 @@
         <v>43</v>
       </c>
       <c r="B45" s="95"/>
-      <c r="C45" s="97"/>
+      <c r="C45" s="97" t="s">
+        <v>44</v>
+      </c>
       <c r="D45" s="97"/>
       <c r="E45" s="4" t="s">
         <v>4</v>
@@ -4026,6 +4023,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="62">
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="C7:F7"/>
@@ -4219,8 +4217,8 @@
   </sheetPr>
   <dimension ref="A1:Z111"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4236,44 +4234,44 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C1" s="44"/>
-      <c r="D1" s="126" t="s">
+      <c r="D1" s="127" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="126"/>
-      <c r="F1" s="126"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="127"/>
       <c r="G1" s="68" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="127" t="s">
+      <c r="H1" s="128" t="s">
         <v>51</v>
       </c>
-      <c r="I1" s="127"/>
-      <c r="J1" s="127"/>
-      <c r="K1" s="127"/>
-      <c r="L1" s="128" t="s">
+      <c r="I1" s="128"/>
+      <c r="J1" s="128"/>
+      <c r="K1" s="128"/>
+      <c r="L1" s="129" t="s">
         <v>52</v>
       </c>
-      <c r="M1" s="128"/>
-      <c r="N1" s="128"/>
-      <c r="O1" s="128"/>
-      <c r="P1" s="128"/>
-      <c r="Q1" s="128"/>
-      <c r="R1" s="128"/>
-      <c r="S1" s="128"/>
-      <c r="T1" s="128"/>
-      <c r="U1" s="128"/>
-      <c r="V1" s="128"/>
-      <c r="W1" s="128"/>
-      <c r="X1" s="128"/>
-      <c r="Y1" s="128"/>
-      <c r="Z1" s="128"/>
+      <c r="M1" s="129"/>
+      <c r="N1" s="129"/>
+      <c r="O1" s="129"/>
+      <c r="P1" s="129"/>
+      <c r="Q1" s="129"/>
+      <c r="R1" s="129"/>
+      <c r="S1" s="129"/>
+      <c r="T1" s="129"/>
+      <c r="U1" s="129"/>
+      <c r="V1" s="129"/>
+      <c r="W1" s="129"/>
+      <c r="X1" s="129"/>
+      <c r="Y1" s="129"/>
+      <c r="Z1" s="129"/>
     </row>
     <row r="2" spans="1:26" s="10" customFormat="1" ht="81" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="46" t="s">
         <v>53</v>
       </c>
       <c r="B2" s="87" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C2" s="46" t="s">
         <v>54</v>
@@ -4285,7 +4283,7 @@
         <v>56</v>
       </c>
       <c r="F2" s="69" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G2" s="70" t="s">
         <v>57</v>
@@ -4306,40 +4304,40 @@
         <v>62</v>
       </c>
       <c r="M2" s="72" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="N2" s="72" t="s">
+        <v>332</v>
+      </c>
+      <c r="O2" s="72" t="s">
         <v>333</v>
       </c>
-      <c r="O2" s="72" t="s">
+      <c r="P2" s="72" t="s">
         <v>334</v>
       </c>
-      <c r="P2" s="72" t="s">
-        <v>335</v>
-      </c>
       <c r="Q2" s="72" t="s">
+        <v>342</v>
+      </c>
+      <c r="R2" s="72" t="s">
         <v>343</v>
       </c>
-      <c r="R2" s="72" t="s">
-        <v>344</v>
-      </c>
       <c r="S2" s="72" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="T2" s="72" t="s">
+        <v>346</v>
+      </c>
+      <c r="U2" s="72" t="s">
         <v>347</v>
       </c>
-      <c r="U2" s="72" t="s">
-        <v>348</v>
-      </c>
       <c r="V2" s="72" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="W2" s="72" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="X2" s="72" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="Y2" s="72" t="s">
         <v>63</v>
@@ -12071,12 +12069,12 @@
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <conditionalFormatting sqref="D1:J98 L3:L98">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="0" priority="3">
       <formula>COUNTIF(D1,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="textLength" errorStyle="warning" operator="greaterThan" allowBlank="1" showErrorMessage="1" error="The Extraction ID cannot be left blank." prompt="Enter the Extraction ID" sqref="F4:F98 D3:F98" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="textLength" errorStyle="warning" operator="greaterThan" allowBlank="1" showErrorMessage="1" error="The Extraction ID cannot be left blank." prompt="Enter the Extraction ID" sqref="D3:E98" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>0</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -12115,7 +12113,7 @@
           <x14:formula1>
             <xm:f>reference!$E$37:$E$39</xm:f>
           </x14:formula1>
-          <xm:sqref>F3</xm:sqref>
+          <xm:sqref>F3:F98</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -12131,7 +12129,7 @@
   <dimension ref="A1:Q39"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -12185,55 +12183,55 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B3">
         <v>30</v>
       </c>
       <c r="C3" s="94" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" t="s">
         <v>271</v>
       </c>
       <c r="I3" s="32" t="s">
+        <v>360</v>
+      </c>
+      <c r="J3" s="32" t="s">
         <v>361</v>
       </c>
-      <c r="J3" s="32" t="s">
-        <v>362</v>
-      </c>
       <c r="L3" s="32" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B4" s="44">
         <v>200</v>
       </c>
       <c r="C4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D4" s="19"/>
       <c r="E4" t="s">
         <v>273</v>
       </c>
       <c r="I4" s="32" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="J4" s="32" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="L4" s="32" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B5" s="44">
         <v>10</v>
@@ -12242,24 +12240,24 @@
         <v>272</v>
       </c>
       <c r="I5" s="32" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="J5" s="32" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="L5" s="32" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B6" s="44">
         <v>800</v>
       </c>
       <c r="C6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E6" s="21" t="s">
         <v>309</v>
@@ -12288,14 +12286,14 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B8">
         <f>ROUND(SUM(flowcell_targetmass/flowcell_maxvol),0)</f>
         <v>67</v>
       </c>
       <c r="C8" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E8">
         <v>50</v>
@@ -12306,13 +12304,13 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B9" s="45" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C9" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="I9" s="32"/>
       <c r="J9" s="32"/>
@@ -12360,10 +12358,10 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
+        <v>379</v>
+      </c>
+      <c r="B13" t="s">
         <v>380</v>
-      </c>
-      <c r="B13" t="s">
-        <v>381</v>
       </c>
       <c r="E13" t="s">
         <v>327</v>
@@ -12399,7 +12397,7 @@
     </row>
     <row r="17" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E17" s="21" t="s">
         <v>330</v>
@@ -12408,25 +12406,22 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
-        <v>331</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E19" t="s">
-        <v>44</v>
-      </c>
       <c r="G19" s="10"/>
       <c r="H19" s="10"/>
     </row>
     <row r="21" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E21" s="80" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F21" s="79"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E22" s="79" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="F22" s="79" t="s">
         <v>266</v>
@@ -12434,100 +12429,100 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F23" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F24" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F25" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="J25" s="10"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F26" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E27" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F27" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F28" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F29" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E32" s="21" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="F32" s="79"/>
     </row>
     <row r="33" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="34" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E34" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="36" spans="5:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E36" s="86" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="37" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E37" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="38" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E38" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="39" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E39" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" selectLockedCells="1"/>
+  <sheetProtection selectLockedCells="1"/>
   <protectedRanges>
     <protectedRange sqref="L3:L9" name="projectlist"/>
     <protectedRange sqref="I3:J9" name="personlist"/>
@@ -12845,7 +12840,7 @@
         <v>287</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>288</v>
@@ -12860,10 +12855,10 @@
         <v>291</v>
       </c>
       <c r="J1" s="10" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="L1" s="10" t="s">
         <v>292</v>
@@ -12929,9 +12924,9 @@
         <f>IF(LEN(exp_summary)=0,"",exp_summary)</f>
         <v/>
       </c>
-      <c r="I2">
+      <c r="I2" t="str">
         <f>IF(LEN(exp_rxns)=0,"",exp_rxns)</f>
-        <v>10</v>
+        <v/>
       </c>
       <c r="J2">
         <v>200</v>
@@ -12962,7 +12957,7 @@
       </c>
       <c r="Q2" t="str">
         <f>IF(LEN(flowcell_chemisty)=0,"",flowcell_chemisty)</f>
-        <v/>
+        <v>R10.4.1</v>
       </c>
       <c r="R2" t="str">
         <f>IF(LEN(flowcell_status)=0,"",flowcell_status)</f>
@@ -13020,7 +13015,7 @@
         <v>303</v>
       </c>
       <c r="C1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D1" t="s">
         <v>284</v>
@@ -13038,7 +13033,7 @@
         <v>307</v>
       </c>
       <c r="I1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Better recording of adaptor ligation volume
</commit_message>
<xml_diff>
--- a/templates/NOMADS_Library_Rapid_Worksheet.xlsx
+++ b/templates/NOMADS_Library_Rapid_Worksheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\warehouse\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA453963-14E5-4A4D-9336-3B264A16102B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE1CF7F-F15C-48B5-AF93-8A582E041D46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="29100" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29670" windowHeight="17370" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assay" sheetId="1" r:id="rId1"/>
@@ -21,34 +21,34 @@
     <sheet name="rxn_metadata" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="adaptlig_rxn_vol">Assay!#REF!</definedName>
-    <definedName name="adaptlig_targetmass">Assay!#REF!</definedName>
-    <definedName name="DNAconc_library">Assay!#REF!</definedName>
+    <definedName name="adaptlig_maxvol_ul">reference!$B$7</definedName>
+    <definedName name="adaptlig_rxn_vol">Assay!$F$27</definedName>
     <definedName name="DNAconc_pooled">Assay!$D$27</definedName>
     <definedName name="endrepair_maxvol">reference!$B$5</definedName>
     <definedName name="exp_date">Assay!$C$2</definedName>
     <definedName name="exp_id">Assay!$C$5</definedName>
     <definedName name="exp_notes">Assay!$C$12</definedName>
     <definedName name="exp_rxns">Assay!$C$11</definedName>
-    <definedName name="exp_subtype">reference!$B$13</definedName>
+    <definedName name="exp_subtype">reference!$B$14</definedName>
     <definedName name="exp_summary">Assay!$C$9</definedName>
-    <definedName name="exp_type">reference!$B$12</definedName>
+    <definedName name="exp_type">reference!$B$13</definedName>
     <definedName name="exp_user">Assay!$C$3</definedName>
-    <definedName name="exp_version">reference!$B$14</definedName>
+    <definedName name="exp_version">reference!$B$15</definedName>
     <definedName name="flowcell_checkpores">Assay!$C$46</definedName>
     <definedName name="flowcell_chemisty">Assay!$C$45</definedName>
     <definedName name="flowcell_id">Assay!$C$42</definedName>
-    <definedName name="flowcell_maxvol">reference!$B$7</definedName>
+    <definedName name="flowcell_maxvol">reference!$B$8</definedName>
     <definedName name="flowcell_runduration">Assay!$C$47</definedName>
     <definedName name="flowcell_status">Assay!$C$43</definedName>
     <definedName name="flowcell_targetmass">reference!$B$6</definedName>
     <definedName name="flowcell_usage_hrs">Assay!$C$44</definedName>
+    <definedName name="library_dna_loaded_ul">Assay!$D$36</definedName>
     <definedName name="library_washbuffer">Assay!#REF!</definedName>
-    <definedName name="Minimum_final_pooled_DNA_conc">reference!$B$8</definedName>
+    <definedName name="Minimum_final_pooled_DNA_conc">reference!$B$9</definedName>
     <definedName name="pcr_product_max_vol">reference!#REF!</definedName>
     <definedName name="pcr_product_targetmass_per_sample">reference!$B$4</definedName>
     <definedName name="seq_platform">Assay!$C$41</definedName>
-    <definedName name="vol_calc">reference!$B$9</definedName>
+    <definedName name="vol_calc">reference!$B$10</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="406">
   <si>
     <t>Date:</t>
   </si>
@@ -1473,9 +1473,6 @@
     <t>Volume of EB to add (µll)</t>
   </si>
   <si>
-    <t>2. Add 1 µl of diluted RA + ADB to the 10 µl of adapter ligated cleaned pooled DNA</t>
-  </si>
-  <si>
     <t>Sequencing Buffer (SB)</t>
   </si>
   <si>
@@ -1486,9 +1483,6 @@
   </si>
   <si>
     <t>sample_type</t>
-  </si>
-  <si>
-    <t>Added Sample type</t>
   </si>
   <si>
     <t>Field</t>
@@ -1541,6 +1535,15 @@
   </si>
   <si>
     <t>Post-PCR clean-up target [DNA]</t>
+  </si>
+  <si>
+    <t>flowcell_massloaded_ng</t>
+  </si>
+  <si>
+    <t>Added total DNA loaded to seq run</t>
+  </si>
+  <si>
+    <t>Adaptor Ligation max volume</t>
   </si>
 </sst>
 </file>
@@ -2585,20 +2588,6 @@
   </cellStyles>
   <dxfs count="34">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF006100"/>
       </font>
@@ -2642,6 +2631,20 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3178,9 +3181,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="tbl_expt_metadata" displayName="tbl_expt_metadata" ref="A1:U2" totalsRowShown="0">
-  <autoFilter ref="A1:U2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="tbl_expt_metadata" displayName="tbl_expt_metadata" ref="A1:V2" totalsRowShown="0">
+  <autoFilter ref="A1:V2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="22">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="expt_id">
       <calculatedColumnFormula>IF(LEN(exp_id)=0,"",exp_id)</calculatedColumnFormula>
     </tableColumn>
@@ -3220,6 +3223,9 @@
     </tableColumn>
     <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name="flowcell_targetmass_ng">
       <calculatedColumnFormula>IF(LEN(flowcell_targetmass)=0,"",flowcell_targetmass)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{7465B1B0-7CCF-4F1B-87AF-E06C52FE6CF9}" name="flowcell_massloaded_ng">
+      <calculatedColumnFormula>IFERROR(SUM(adaptlig_rxn_vol*DNAconc_pooled), "")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="flowcell_maxvol_ul">
       <calculatedColumnFormula>IF(LEN(flowcell_maxvol)=0,"",flowcell_maxvol)</calculatedColumnFormula>
@@ -3453,8 +3459,8 @@
   </sheetPr>
   <dimension ref="A1:Q47"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47:D47"/>
+    <sheetView topLeftCell="A24" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27:G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3802,7 +3808,7 @@
     </row>
     <row r="25" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -3849,12 +3855,12 @@
       </c>
       <c r="E27" s="104"/>
       <c r="F27" s="105" t="str">
-        <f>IFERROR(IF(SUM(flowcell_targetmass/DNAconc_pooled)&gt;flowcell_maxvol-1,flowcell_maxvol-1, SUM(flowcell_targetmass/DNAconc_pooled)),"")</f>
+        <f>IFERROR(IF(SUM(flowcell_targetmass/DNAconc_pooled)&gt;adaptlig_maxvol_ul,adaptlig_maxvol_ul, SUM(flowcell_targetmass/DNAconc_pooled)),"")</f>
         <v/>
       </c>
       <c r="G27" s="105"/>
       <c r="H27" s="109" t="str">
-        <f>IFERROR(SUM(11-F27),"")</f>
+        <f>IFERROR(SUM(adaptlig_maxvol_ul-F27),"")</f>
         <v/>
       </c>
       <c r="I27" s="109"/>
@@ -3873,8 +3879,9 @@
       <c r="G30" s="4"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
-        <v>389</v>
+      <c r="A31" s="8" t="str">
+        <f>_xlfn.CONCAT("2. Add 1 µl of diluted RA + ADB to the ", adaptlig_maxvol_ul, " µl of adapter ligated cleaned pooled DNA")</f>
+        <v>2. Add 1 µl of diluted RA + ADB to the 10 µl of adapter ligated cleaned pooled DNA</v>
       </c>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
@@ -3911,13 +3918,14 @@
       <c r="B36" s="103"/>
       <c r="C36" s="103"/>
       <c r="D36" s="108">
+        <f>flowcell_maxvol</f>
         <v>11</v>
       </c>
       <c r="E36" s="108"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="100" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B37" s="100"/>
       <c r="C37" s="100"/>
@@ -3928,7 +3936,7 @@
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="100" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B38" s="100"/>
       <c r="C38" s="100"/>
@@ -4089,15 +4097,15 @@
     <mergeCell ref="C45:D45"/>
   </mergeCells>
   <conditionalFormatting sqref="C2:C4 C7:C8 C11:C12 B27:C27 C41:C43 C45:C47">
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="5" priority="7">
       <formula>COUNTIF(B2,"")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C46">
-    <cfRule type="cellIs" dxfId="5" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="8" operator="lessThan">
       <formula>800</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="9" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="9" operator="greaterThanOrEqual">
       <formula>800</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4133,7 +4141,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="12" operator="lessThan" id="{19D8DF94-2AE3-467C-A57C-35B04CD0367F}">
-            <xm:f>reference!$B$8</xm:f>
+            <xm:f>reference!$B$9</xm:f>
             <x14:dxf>
               <font>
                 <color rgb="FF9C0006"/>
@@ -4146,7 +4154,7 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="cellIs" priority="13" operator="greaterThanOrEqual" id="{840A6DF8-F522-46F8-ADCF-F799D761F007}">
-            <xm:f>reference!$B$8</xm:f>
+            <xm:f>reference!$B$9</xm:f>
             <x14:dxf>
               <font>
                 <color rgb="FF006100"/>
@@ -4283,7 +4291,7 @@
         <v>56</v>
       </c>
       <c r="F2" s="69" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G2" s="70" t="s">
         <v>57</v>
@@ -12069,7 +12077,7 @@
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <conditionalFormatting sqref="D1:J98 L3:L98">
-    <cfRule type="expression" dxfId="0" priority="3">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>COUNTIF(D1,"")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12129,7 +12137,7 @@
   <dimension ref="A1:Q39"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -12183,13 +12191,13 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B3">
         <v>30</v>
       </c>
       <c r="C3" s="94" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" t="s">
@@ -12202,7 +12210,7 @@
         <v>361</v>
       </c>
       <c r="L3" s="32" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -12226,7 +12234,7 @@
         <v>362</v>
       </c>
       <c r="L4" s="32" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -12246,7 +12254,7 @@
         <v>363</v>
       </c>
       <c r="L5" s="32" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="6" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -12269,10 +12277,10 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>276</v>
+        <v>405</v>
       </c>
       <c r="B7" s="44">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
         <v>272</v>
@@ -12286,14 +12294,13 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>402</v>
-      </c>
-      <c r="B8">
-        <f>ROUND(SUM(flowcell_targetmass/flowcell_maxvol),0)</f>
-        <v>67</v>
+        <v>276</v>
+      </c>
+      <c r="B8" s="44">
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>403</v>
+        <v>272</v>
       </c>
       <c r="E8">
         <v>50</v>
@@ -12304,19 +12311,29 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>377</v>
-      </c>
-      <c r="B9" s="45" t="s">
-        <v>339</v>
+        <v>400</v>
+      </c>
+      <c r="B9">
+        <f>ROUND(SUM(flowcell_targetmass/flowcell_maxvol),0)</f>
+        <v>73</v>
       </c>
       <c r="C9" t="s">
-        <v>359</v>
+        <v>401</v>
       </c>
       <c r="I9" s="32"/>
       <c r="J9" s="32"/>
       <c r="L9" s="32"/>
     </row>
     <row r="10" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>377</v>
+      </c>
+      <c r="B10" s="45" t="s">
+        <v>339</v>
+      </c>
+      <c r="C10" t="s">
+        <v>359</v>
+      </c>
       <c r="E10" s="21" t="s">
         <v>325</v>
       </c>
@@ -12325,12 +12342,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="20" t="s">
-        <v>279</v>
-      </c>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
         <v>38</v>
       </c>
@@ -12338,13 +12350,12 @@
         <v>275</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>281</v>
-      </c>
-      <c r="B12" t="s">
-        <v>282</v>
-      </c>
+    <row r="12" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="20" t="s">
+        <v>279</v>
+      </c>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
       <c r="E12" t="s">
         <v>326</v>
       </c>
@@ -12358,10 +12369,10 @@
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>379</v>
+        <v>281</v>
       </c>
       <c r="B13" t="s">
-        <v>380</v>
+        <v>282</v>
       </c>
       <c r="E13" t="s">
         <v>327</v>
@@ -12372,10 +12383,10 @@
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>283</v>
-      </c>
-      <c r="B14">
-        <v>2</v>
+        <v>379</v>
+      </c>
+      <c r="B14" t="s">
+        <v>380</v>
       </c>
       <c r="E14" t="s">
         <v>328</v>
@@ -12385,19 +12396,20 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>283</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
       <c r="E15" s="10" t="s">
         <v>329</v>
       </c>
       <c r="F15" s="10"/>
     </row>
-    <row r="16" spans="1:17" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="20" t="s">
+    <row r="17" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="20" t="s">
         <v>308</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="10" t="s">
-        <v>394</v>
       </c>
       <c r="E17" s="21" t="s">
         <v>330</v>
@@ -12405,6 +12417,9 @@
       <c r="F17" s="79"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>404</v>
+      </c>
       <c r="E18" t="s">
         <v>44</v>
       </c>
@@ -12503,22 +12518,22 @@
     </row>
     <row r="36" spans="5:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E36" s="86" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="37" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E37" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="38" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E38" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="39" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E39" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
   </sheetData>
@@ -12528,7 +12543,7 @@
     <protectedRange sqref="I3:J9" name="personlist"/>
   </protectedRanges>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9" xr:uid="{5103F0B0-5A7D-4213-9279-0C438FB60721}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B10" xr:uid="{5103F0B0-5A7D-4213-9279-0C438FB60721}">
       <formula1>$E$23:$E$29</formula1>
     </dataValidation>
   </dataValidations>
@@ -12812,10 +12827,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -12826,7 +12841,7 @@
     <col min="11" max="11" width="12.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="10" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="10" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>284</v>
       </c>
@@ -12870,28 +12885,31 @@
         <v>294</v>
       </c>
       <c r="O1" s="10" t="s">
+        <v>403</v>
+      </c>
+      <c r="P1" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="Q1" s="10" t="s">
         <v>296</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="R1" s="10" t="s">
         <v>297</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="S1" s="10" t="s">
         <v>298</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="T1" s="10" t="s">
         <v>299</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="U1" s="10" t="s">
         <v>300</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="V1" s="10" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>IF(LEN(exp_id)=0,"",exp_id)</f>
         <v/>
@@ -12914,7 +12932,7 @@
       </c>
       <c r="F2">
         <f>IF(LEN(exp_version)=0,"",exp_version)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G2" t="str">
         <f>IF(LEN(exp_notes)=0,"",exp_notes)</f>
@@ -12947,37 +12965,41 @@
         <f>IF(LEN(flowcell_targetmass)=0,"",flowcell_targetmass)</f>
         <v>800</v>
       </c>
-      <c r="O2">
+      <c r="O2" t="str">
+        <f>IFERROR(SUM(adaptlig_rxn_vol*DNAconc_pooled), "")</f>
+        <v/>
+      </c>
+      <c r="P2">
         <f>IF(LEN(flowcell_maxvol)=0,"",flowcell_maxvol)</f>
-        <v>12</v>
-      </c>
-      <c r="P2" t="str">
+        <v>11</v>
+      </c>
+      <c r="Q2" t="str">
         <f>IF(LEN(flowcell_id)=0,"",flowcell_id)</f>
         <v/>
       </c>
-      <c r="Q2" t="str">
+      <c r="R2" t="str">
         <f>IF(LEN(flowcell_chemisty)=0,"",flowcell_chemisty)</f>
         <v>R10.4.1</v>
       </c>
-      <c r="R2" t="str">
+      <c r="S2" t="str">
         <f>IF(LEN(flowcell_status)=0,"",flowcell_status)</f>
         <v/>
       </c>
-      <c r="S2" t="str">
+      <c r="T2" t="str">
         <f>IF(LEN(flowcell_checkpores)=0,"",flowcell_checkpores)</f>
         <v/>
       </c>
-      <c r="T2" t="str">
+      <c r="U2" t="str">
         <f>IF(LEN(flowcell_runduration)=0,"",flowcell_runduration)</f>
         <v/>
       </c>
-      <c r="U2" t="str">
+      <c r="V2" t="str">
         <f>IF(LEN(flowcell_usage_hrs)=0,"",flowcell_usage_hrs)</f>
         <v/>
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="XAJEfl/fMWsRVHvgk+FWJqIpzpTZj0cfsa5tnX61QDmOAkNCaevskOhYzzx78yqZyb8IoUCjTXL/rN2ecJ815w==" saltValue="ckH/95JzUMCShg6iv4fF3Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="alLNTrutkK14cWSVMZVhqZfkCZ1TmxaRWiW1DyoF0dM9zpbX9Q6JVsn6+AiK7UnsFzFw7DP140vekGlMaOYG1A==" saltValue="8gA+5GoCd81DFGgH+LfSfw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <tableParts count="1">
@@ -13015,7 +13037,7 @@
         <v>303</v>
       </c>
       <c r="C1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D1" t="s">
         <v>284</v>

</xml_diff>

<commit_message>
Better instructions and some corrections
</commit_message>
<xml_diff>
--- a/templates/NOMADS_Library_Rapid_Worksheet.xlsx
+++ b/templates/NOMADS_Library_Rapid_Worksheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\git\warehouse\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{075F63ED-992C-4E32-B37B-6FA5790B1B19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E88A3EF-AC8C-4710-86B3-70268096DC63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46284" windowHeight="23172" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="27288" windowHeight="17532" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assay" sheetId="1" r:id="rId1"/>
@@ -33,21 +33,21 @@
     <definedName name="exp_type">Reference!$B$27</definedName>
     <definedName name="exp_user">Assay!$C$3</definedName>
     <definedName name="exp_version">Reference!$B$29</definedName>
-    <definedName name="flowcell_checkpores">Assay!$C$46</definedName>
-    <definedName name="flowcell_chemisty">Assay!$C$45</definedName>
-    <definedName name="flowcell_id">Assay!$C$42</definedName>
+    <definedName name="flowcell_checkpores">Assay!$C$35</definedName>
+    <definedName name="flowcell_chemisty">Assay!$C$54</definedName>
+    <definedName name="flowcell_id">Assay!$C$51</definedName>
     <definedName name="flowcell_maxvol">Reference!$B$22</definedName>
-    <definedName name="flowcell_runduration">Assay!$C$47</definedName>
-    <definedName name="flowcell_status">Assay!$C$43</definedName>
+    <definedName name="flowcell_runduration">Assay!$C$55</definedName>
+    <definedName name="flowcell_status">Assay!$C$52</definedName>
     <definedName name="flowcell_targetmass">Reference!$B$20</definedName>
-    <definedName name="flowcell_usage_hrs">Assay!$C$44</definedName>
-    <definedName name="library_dna_loaded_ul">Assay!$D$36</definedName>
+    <definedName name="flowcell_usage_hrs">Assay!$C$53</definedName>
+    <definedName name="library_dna_loaded_ul">Assay!$D$43</definedName>
     <definedName name="library_washbuffer">Assay!#REF!</definedName>
     <definedName name="Minimum_final_pooled_DNA_conc">Reference!$B$23</definedName>
     <definedName name="pcr_product_max_vol">Reference!#REF!</definedName>
     <definedName name="pcr_product_targetmass_per_sample">Reference!$B$18</definedName>
     <definedName name="Post_PCR_target_DNA_conc">Reference!$B$17</definedName>
-    <definedName name="seq_platform">Assay!$C$41</definedName>
+    <definedName name="seq_platform">Assay!$C$50</definedName>
     <definedName name="vol_calc">Reference!$B$24</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="398">
   <si>
     <t>Date:</t>
   </si>
@@ -234,9 +234,6 @@
     <t>(ensure mixed thoroughly just before addition)</t>
   </si>
   <si>
-    <t>Sequencing Run Details</t>
-  </si>
-  <si>
     <t>Platform:</t>
   </si>
   <si>
@@ -1184,9 +1181,6 @@
     <t>3. Incubate for 5 min at RT</t>
   </si>
   <si>
-    <t>1. Combine 1.5 µl Rapid Adaptor (RA) and 3.5 µl Adaptor Buffer (ADB) in fresh tube</t>
-  </si>
-  <si>
     <t>2. Add 1 µl of rapid barcode to each sample, mix thoroughly and incubate:</t>
   </si>
   <si>
@@ -1220,19 +1214,10 @@
     <t>Flow cell target mass</t>
   </si>
   <si>
-    <t>Volume to adaptor ligate (µll)</t>
-  </si>
-  <si>
     <t>Person B</t>
   </si>
   <si>
     <t>Person C</t>
-  </si>
-  <si>
-    <t>4 - Loading Library</t>
-  </si>
-  <si>
-    <t>Volume of EB to add (µll)</t>
   </si>
   <si>
     <t>Sequencing Buffer (SB)</t>
@@ -1439,6 +1424,42 @@
   </si>
   <si>
     <t>Combined Instructions into Reference sheet</t>
+  </si>
+  <si>
+    <t>Volume to adaptor ligate (µl)</t>
+  </si>
+  <si>
+    <t>Volume of EB to add (µl)</t>
+  </si>
+  <si>
+    <t>1. Combine 1 µl Rapid Adaptor (RA) and 2.3 µl Adaptor Buffer (ADB) in fresh tube</t>
+  </si>
+  <si>
+    <t>4 - Flow cell prep</t>
+  </si>
+  <si>
+    <t>1. Mix 1,170 µl Flow Cell Flush (FCF) with 30 µl Flow Cell Tether (FCT)</t>
+  </si>
+  <si>
+    <t>2. Open priming  port and aspirate (by scrolling) with a P1000 set to 200 µl to remove any bubbles</t>
+  </si>
+  <si>
+    <t>3. Add 800 µl of the priming mix to the priming port and incubate for 5 mins</t>
+  </si>
+  <si>
+    <t>4. Open Spot-On port and add 200 µl of the priming mix to the priming port</t>
+  </si>
+  <si>
+    <t>Prepare library and load all 75 µl dropwise to the spot-on port</t>
+  </si>
+  <si>
+    <t>5 - Library Loading</t>
+  </si>
+  <si>
+    <t>6. Sequencing</t>
+  </si>
+  <si>
+    <t>In minknow select 'SQK-RBK114-96' kit with 'Super accurate basecalling'</t>
   </si>
 </sst>
 </file>
@@ -2055,7 +2076,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -2329,6 +2350,12 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
@@ -2361,7 +2388,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -2374,7 +2401,7 @@
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -2506,6 +2533,13 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF006100"/>
       </font>
@@ -2522,13 +2556,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3493,10 +3520,10 @@
     <tabColor rgb="FF92D050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q47"/>
+  <dimension ref="A1:Q55"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:F2"/>
+    <sheetView topLeftCell="A26" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3505,171 +3532,171 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="117" t="s">
-        <v>335</v>
-      </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="117"/>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="117"/>
-      <c r="G1" s="117"/>
-      <c r="H1" s="117"/>
-      <c r="I1" s="117"/>
-      <c r="J1" s="117"/>
-      <c r="K1" s="117"/>
-      <c r="L1" s="117"/>
+      <c r="A1" s="119" t="s">
+        <v>334</v>
+      </c>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
+      <c r="H1" s="119"/>
+      <c r="I1" s="119"/>
+      <c r="J1" s="119"/>
+      <c r="K1" s="119"/>
+      <c r="L1" s="119"/>
     </row>
     <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="91" t="s">
+      <c r="A2" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="91"/>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="98" t="s">
+      <c r="B2" s="93"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="120"/>
+      <c r="G2" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="98"/>
-      <c r="J2" s="119" t="s">
+      <c r="H2" s="100"/>
+      <c r="J2" s="121" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="119"/>
+      <c r="K2" s="121"/>
     </row>
     <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="91" t="s">
+      <c r="A3" s="93" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="91"/>
-      <c r="C3" s="120"/>
-      <c r="D3" s="120"/>
-      <c r="E3" s="120"/>
-      <c r="F3" s="120"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="122"/>
+      <c r="D3" s="122"/>
+      <c r="E3" s="122"/>
+      <c r="F3" s="122"/>
       <c r="G3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="121" t="s">
+      <c r="J3" s="123" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="121"/>
+      <c r="K3" s="123"/>
     </row>
     <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="91" t="s">
+      <c r="A4" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="91"/>
-      <c r="C4" s="118"/>
-      <c r="D4" s="118"/>
-      <c r="E4" s="118"/>
-      <c r="F4" s="118"/>
+      <c r="B4" s="93"/>
+      <c r="C4" s="120"/>
+      <c r="D4" s="120"/>
+      <c r="E4" s="120"/>
+      <c r="F4" s="120"/>
       <c r="G4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="122" t="s">
+      <c r="J4" s="124" t="s">
         <v>8</v>
       </c>
-      <c r="K4" s="122"/>
+      <c r="K4" s="124"/>
     </row>
     <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="108" t="s">
+      <c r="A5" s="110" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="108"/>
-      <c r="C5" s="106" t="str">
+      <c r="B5" s="110"/>
+      <c r="C5" s="108" t="str">
         <f>IF(OR(ISBLANK(C3),ISBLANK(C4)),"",CONCATENATE("SL",VLOOKUP(C3,Reference!I17:J26,2,FALSE()),C4))</f>
         <v/>
       </c>
-      <c r="D5" s="106"/>
-      <c r="E5" s="106"/>
-      <c r="F5" s="106"/>
+      <c r="D5" s="108"/>
+      <c r="E5" s="108"/>
+      <c r="F5" s="108"/>
       <c r="G5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="107" t="s">
+      <c r="J5" s="109" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="107"/>
+      <c r="K5" s="109"/>
     </row>
     <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="108" t="s">
+      <c r="A6" s="110" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="108"/>
-      <c r="C6" s="109" t="str">
+      <c r="B6" s="110"/>
+      <c r="C6" s="111" t="str">
         <f>IF(OR(ISBLANK(C2),ISBLANK(C3),ISBLANK(C4)),"",CONCATENATE(C2,"_SeqLib_",C5))</f>
         <v/>
       </c>
-      <c r="D6" s="109"/>
-      <c r="E6" s="109"/>
-      <c r="F6" s="109"/>
+      <c r="D6" s="111"/>
+      <c r="E6" s="111"/>
+      <c r="F6" s="111"/>
       <c r="G6" s="4"/>
-      <c r="J6" s="107"/>
-      <c r="K6" s="107"/>
+      <c r="J6" s="109"/>
+      <c r="K6" s="109"/>
     </row>
     <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="115" t="s">
+      <c r="A7" s="117" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="115"/>
-      <c r="C7" s="116"/>
-      <c r="D7" s="116"/>
-      <c r="E7" s="116"/>
-      <c r="F7" s="116"/>
+      <c r="B7" s="117"/>
+      <c r="C7" s="118"/>
+      <c r="D7" s="118"/>
+      <c r="E7" s="118"/>
+      <c r="F7" s="118"/>
       <c r="G7" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="115" t="s">
+      <c r="A8" s="117" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="115"/>
-      <c r="C8" s="116"/>
-      <c r="D8" s="116"/>
-      <c r="E8" s="116"/>
-      <c r="F8" s="116"/>
+      <c r="B8" s="117"/>
+      <c r="C8" s="118"/>
+      <c r="D8" s="118"/>
+      <c r="E8" s="118"/>
+      <c r="F8" s="118"/>
       <c r="G8" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="111" t="s">
+      <c r="A9" s="113" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="111"/>
-      <c r="C9" s="112" t="str">
+      <c r="B9" s="113"/>
+      <c r="C9" s="114" t="str">
         <f>IF(OR(LEN(C7)=0, LEN(C8)=0),"",CONCATENATE(C7,"_Batch",C8))</f>
         <v/>
       </c>
-      <c r="D9" s="112"/>
-      <c r="E9" s="112"/>
-      <c r="F9" s="112"/>
+      <c r="D9" s="114"/>
+      <c r="E9" s="114"/>
+      <c r="F9" s="114"/>
       <c r="G9" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="111" t="s">
+      <c r="A10" s="113" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="111"/>
-      <c r="C10" s="112" t="str">
+      <c r="B10" s="113"/>
+      <c r="C10" s="114" t="str">
         <f>IF(OR(LEN(C6)=0,LEN(exp_summary)=0),"",CONCATENATE(C6,"_",exp_summary))</f>
         <v/>
       </c>
-      <c r="D10" s="112"/>
-      <c r="E10" s="112"/>
-      <c r="F10" s="112"/>
-      <c r="G10" s="112"/>
-      <c r="H10" s="112"/>
+      <c r="D10" s="114"/>
+      <c r="E10" s="114"/>
+      <c r="F10" s="114"/>
+      <c r="G10" s="114"/>
+      <c r="H10" s="114"/>
     </row>
     <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="91" t="s">
+      <c r="A11" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="91"/>
+      <c r="B11" s="93"/>
       <c r="C11" s="25"/>
       <c r="D11" s="23"/>
       <c r="E11" s="23"/>
@@ -3677,32 +3704,32 @@
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="91" t="s">
+      <c r="A12" s="93" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="91"/>
-      <c r="C12" s="113"/>
-      <c r="D12" s="113"/>
-      <c r="E12" s="113"/>
-      <c r="F12" s="113"/>
-      <c r="G12" s="113"/>
-      <c r="H12" s="113"/>
-      <c r="I12" s="113"/>
-      <c r="J12" s="113"/>
-      <c r="K12" s="113"/>
+      <c r="B12" s="93"/>
+      <c r="C12" s="115"/>
+      <c r="D12" s="115"/>
+      <c r="E12" s="115"/>
+      <c r="F12" s="115"/>
+      <c r="G12" s="115"/>
+      <c r="H12" s="115"/>
+      <c r="I12" s="115"/>
+      <c r="J12" s="115"/>
+      <c r="K12" s="115"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="113"/>
-      <c r="D13" s="113"/>
-      <c r="E13" s="113"/>
-      <c r="F13" s="113"/>
-      <c r="G13" s="113"/>
-      <c r="H13" s="113"/>
-      <c r="I13" s="113"/>
-      <c r="J13" s="113"/>
-      <c r="K13" s="113"/>
+      <c r="C13" s="115"/>
+      <c r="D13" s="115"/>
+      <c r="E13" s="115"/>
+      <c r="F13" s="115"/>
+      <c r="G13" s="115"/>
+      <c r="H13" s="115"/>
+      <c r="I13" s="115"/>
+      <c r="J13" s="115"/>
+      <c r="K13" s="115"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C14" s="5"/>
@@ -3725,25 +3752,25 @@
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="H16" s="4"/>
-      <c r="I16" s="114" t="s">
+      <c r="I16" s="116" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="114"/>
-      <c r="K16" s="114"/>
+      <c r="J16" s="116"/>
+      <c r="K16" s="116"/>
     </row>
     <row r="17" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="G17" s="8"/>
-      <c r="I17" s="95" t="s">
+      <c r="I17" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="J17" s="95"/>
+      <c r="J17" s="97"/>
       <c r="K17" s="9" t="s">
         <v>26</v>
       </c>
@@ -3755,10 +3782,10 @@
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="G18" s="8"/>
-      <c r="I18" s="110">
+      <c r="I18" s="112">
         <v>30</v>
       </c>
-      <c r="J18" s="110"/>
+      <c r="J18" s="112"/>
       <c r="K18" s="2" t="s">
         <v>27</v>
       </c>
@@ -3770,10 +3797,10 @@
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="G19" s="8"/>
-      <c r="I19" s="110">
+      <c r="I19" s="112">
         <v>30</v>
       </c>
-      <c r="J19" s="110"/>
+      <c r="J19" s="112"/>
       <c r="K19" s="7">
         <v>2</v>
       </c>
@@ -3785,10 +3812,10 @@
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="G20" s="8"/>
-      <c r="I20" s="110">
+      <c r="I20" s="112">
         <v>80</v>
       </c>
-      <c r="J20" s="110"/>
+      <c r="J20" s="112"/>
       <c r="K20" s="2">
         <v>2</v>
       </c>
@@ -3800,10 +3827,10 @@
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="G21" s="8"/>
-      <c r="I21" s="110">
+      <c r="I21" s="112">
         <v>8</v>
       </c>
-      <c r="J21" s="110"/>
+      <c r="J21" s="112"/>
       <c r="K21" s="2" t="s">
         <v>27</v>
       </c>
@@ -3816,7 +3843,7 @@
     </row>
     <row r="23" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -3826,25 +3853,25 @@
       <c r="G23" s="24"/>
     </row>
     <row r="24" spans="1:17" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="98" t="str">
+      <c r="A24" s="100" t="str">
         <f>_xlfn.CONCAT("2. Clean up: Add 0.5x vol (", SUM(5*exp_rxns)*0.5,"µl) AMPPure beads for 5 min RT with mixing, wash with fresh 80% EtOH, spin, dry, re-suspend in 15 µl EB (10 min @RT) and transfer eluate to fresh tube")</f>
         <v>2. Clean up: Add 0.5x vol (0µl) AMPPure beads for 5 min RT with mixing, wash with fresh 80% EtOH, spin, dry, re-suspend in 15 µl EB (10 min @RT) and transfer eluate to fresh tube</v>
       </c>
-      <c r="B24" s="98"/>
-      <c r="C24" s="98"/>
-      <c r="D24" s="98"/>
-      <c r="E24" s="98"/>
-      <c r="F24" s="98"/>
-      <c r="G24" s="98"/>
-      <c r="H24" s="98"/>
-      <c r="I24" s="98"/>
-      <c r="J24" s="98"/>
-      <c r="K24" s="98"/>
-      <c r="L24" s="98"/>
+      <c r="B24" s="100"/>
+      <c r="C24" s="100"/>
+      <c r="D24" s="100"/>
+      <c r="E24" s="100"/>
+      <c r="F24" s="100"/>
+      <c r="G24" s="100"/>
+      <c r="H24" s="100"/>
+      <c r="I24" s="100"/>
+      <c r="J24" s="100"/>
+      <c r="K24" s="100"/>
+      <c r="L24" s="100"/>
     </row>
     <row r="25" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -3863,43 +3890,45 @@
       <c r="C26" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="99" t="s">
+      <c r="D26" s="101" t="s">
         <v>32</v>
       </c>
-      <c r="E26" s="99"/>
-      <c r="F26" s="102" t="s">
-        <v>351</v>
-      </c>
-      <c r="G26" s="102"/>
-      <c r="H26" s="102" t="s">
-        <v>355</v>
-      </c>
-      <c r="I26" s="102"/>
+      <c r="E26" s="101"/>
+      <c r="F26" s="104" t="s">
+        <v>386</v>
+      </c>
+      <c r="G26" s="104"/>
+      <c r="H26" s="104" t="s">
+        <v>387</v>
+      </c>
+      <c r="I26" s="104"/>
     </row>
     <row r="27" spans="1:17" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A27" s="12">
         <f>SUM(exp_rxns*5)*0.5</f>
         <v>0</v>
       </c>
-      <c r="B27" s="28"/>
+      <c r="B27" s="28">
+        <v>14.6</v>
+      </c>
       <c r="C27" s="28">
         <v>10</v>
       </c>
-      <c r="D27" s="100">
+      <c r="D27" s="102">
         <f>SUM(B27*C27)</f>
-        <v>0</v>
-      </c>
-      <c r="E27" s="100"/>
-      <c r="F27" s="101" t="str">
-        <f>IFERROR(IF(SUM(flowcell_targetmass/DNAconc_pooled)&gt;adaptlig_maxvol_ul,adaptlig_maxvol_ul, SUM(flowcell_targetmass/DNAconc_pooled)),"")</f>
-        <v/>
-      </c>
-      <c r="G27" s="101"/>
-      <c r="H27" s="105" t="str">
+        <v>146</v>
+      </c>
+      <c r="E27" s="102"/>
+      <c r="F27" s="103">
+        <f>IFERROR(IF(SUM(flowcell_targetmass/DNAconc_pooled)&gt;adaptlig_maxvol_ul,adaptlig_maxvol_ul, ROUNDUP(SUM(flowcell_targetmass/DNAconc_pooled),1)),"")</f>
+        <v>5.5</v>
+      </c>
+      <c r="G27" s="103"/>
+      <c r="H27" s="107">
         <f>IFERROR(SUM(adaptlig_maxvol_ul-F27),"")</f>
-        <v/>
-      </c>
-      <c r="I27" s="105"/>
+        <v>4.5</v>
+      </c>
+      <c r="I27" s="107"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="6" t="s">
@@ -3908,7 +3937,7 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>339</v>
+        <v>388</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -3924,7 +3953,7 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
@@ -3933,142 +3962,185 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="95" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="93" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" s="93"/>
+      <c r="C35" s="94">
+        <v>234</v>
+      </c>
+      <c r="D35" s="94"/>
+      <c r="E35" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="8" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="8" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="8" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="8" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="6" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="97" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="95"/>
-      <c r="C35" s="95"/>
-      <c r="D35" s="103" t="s">
+      <c r="B42" s="97"/>
+      <c r="C42" s="97"/>
+      <c r="D42" s="105" t="s">
         <v>24</v>
       </c>
-      <c r="E35" s="103"/>
-    </row>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="99" t="s">
+      <c r="E42" s="105"/>
+    </row>
+    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="99"/>
-      <c r="C36" s="99"/>
-      <c r="D36" s="104">
+      <c r="B43" s="101"/>
+      <c r="C43" s="101"/>
+      <c r="D43" s="106">
         <f>flowcell_maxvol</f>
         <v>11</v>
       </c>
-      <c r="E36" s="104"/>
-    </row>
-    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="96" t="s">
-        <v>356</v>
-      </c>
-      <c r="B37" s="96"/>
-      <c r="C37" s="96"/>
-      <c r="D37" s="97">
+      <c r="E43" s="106"/>
+    </row>
+    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="98" t="s">
+        <v>351</v>
+      </c>
+      <c r="B44" s="98"/>
+      <c r="C44" s="98"/>
+      <c r="D44" s="99">
         <v>37.5</v>
       </c>
-      <c r="E37" s="97"/>
-    </row>
-    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="96" t="s">
-        <v>357</v>
-      </c>
-      <c r="B38" s="96"/>
-      <c r="C38" s="96"/>
-      <c r="D38" s="97">
+      <c r="E44" s="99"/>
+    </row>
+    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="98" t="s">
+        <v>352</v>
+      </c>
+      <c r="B45" s="98"/>
+      <c r="C45" s="98"/>
+      <c r="D45" s="99">
         <v>25.5</v>
       </c>
-      <c r="E38" s="97"/>
-      <c r="F38" s="4" t="s">
+      <c r="E45" s="99"/>
+      <c r="F45" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="6" t="s">
+    <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="B46" s="91"/>
+      <c r="C46" s="91"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="C48" s="4"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49" s="92" t="s">
+        <v>397</v>
+      </c>
+      <c r="C49" s="4"/>
+    </row>
+    <row r="50" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="93" t="s">
         <v>36</v>
       </c>
-      <c r="C40" s="4"/>
-    </row>
-    <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="91" t="s">
+      <c r="B50" s="93"/>
+      <c r="C50" s="95" t="s">
         <v>37</v>
       </c>
-      <c r="B41" s="91"/>
-      <c r="C41" s="93" t="s">
+      <c r="D50" s="95"/>
+      <c r="E50" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="93" t="s">
         <v>38</v>
       </c>
-      <c r="D41" s="93"/>
-      <c r="E41" s="4" t="s">
+      <c r="B51" s="93"/>
+      <c r="C51" s="94"/>
+      <c r="D51" s="94"/>
+    </row>
+    <row r="52" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="93" t="s">
+        <v>39</v>
+      </c>
+      <c r="B52" s="93"/>
+      <c r="C52" s="94"/>
+      <c r="D52" s="94"/>
+      <c r="E52" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="91" t="s">
-        <v>39</v>
-      </c>
-      <c r="B42" s="91"/>
-      <c r="C42" s="92"/>
-      <c r="D42" s="92"/>
-    </row>
-    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="91" t="s">
+    <row r="53" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="93" t="s">
         <v>40</v>
       </c>
-      <c r="B43" s="91"/>
-      <c r="C43" s="92"/>
-      <c r="D43" s="92"/>
-      <c r="E43" s="4" t="s">
+      <c r="B53" s="93"/>
+      <c r="C53" s="96" t="str">
+        <f>IF(flowcell_status="New",0,"")</f>
+        <v/>
+      </c>
+      <c r="D53" s="96"/>
+      <c r="E53" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="93" t="s">
+        <v>42</v>
+      </c>
+      <c r="B54" s="93"/>
+      <c r="C54" s="95" t="s">
+        <v>43</v>
+      </c>
+      <c r="D54" s="95"/>
+      <c r="E54" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="91" t="s">
-        <v>41</v>
-      </c>
-      <c r="B44" s="91"/>
-      <c r="C44" s="94" t="str">
-        <f>IF(flowcell_status="New",0,"")</f>
-        <v/>
-      </c>
-      <c r="D44" s="94"/>
-      <c r="E44" s="8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="91" t="s">
-        <v>43</v>
-      </c>
-      <c r="B45" s="91"/>
-      <c r="C45" s="93" t="s">
-        <v>44</v>
-      </c>
-      <c r="D45" s="93"/>
-      <c r="E45" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="91" t="s">
-        <v>45</v>
-      </c>
-      <c r="B46" s="91"/>
-      <c r="C46" s="92"/>
-      <c r="D46" s="92"/>
-      <c r="E46" s="8" t="s">
+    <row r="55" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="93" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="91" t="s">
+      <c r="B55" s="93"/>
+      <c r="C55" s="94"/>
+      <c r="D55" s="94"/>
+      <c r="E55" s="8" t="s">
         <v>47</v>
-      </c>
-      <c r="B47" s="91"/>
-      <c r="C47" s="92"/>
-      <c r="D47" s="92"/>
-      <c r="E47" s="8" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -4107,46 +4179,46 @@
     <mergeCell ref="C12:K13"/>
     <mergeCell ref="I16:K16"/>
     <mergeCell ref="I17:J17"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="A45:C45"/>
+    <mergeCell ref="D45:E45"/>
     <mergeCell ref="A24:L24"/>
     <mergeCell ref="D26:E26"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="F27:G27"/>
     <mergeCell ref="F26:G26"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="D43:E43"/>
     <mergeCell ref="H26:I26"/>
     <mergeCell ref="H27:I27"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="C45:D45"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="C35:D35"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="C55:D55"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="C53:D53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="C54:D54"/>
   </mergeCells>
-  <conditionalFormatting sqref="C2:C4 C7:C8 C11:C12 B27:C27 C41:C43 C45:C47">
+  <conditionalFormatting sqref="C2:C4 C7:C8 C11:C12 B27:C27 C35 C50:C52 C54:C55">
     <cfRule type="expression" dxfId="9" priority="7">
       <formula>COUNTIF(B2,"")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C46">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="lessThan">
+  <conditionalFormatting sqref="C35">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="lessThan">
       <formula>800</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="7" priority="9" operator="greaterThanOrEqual">
       <formula>800</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4169,7 +4241,7 @@
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="14" id="{7D748971-4ED9-4DAD-A430-377FADB0435A}">
-            <xm:f>COUNTIF($C$43,Reference!$E$18)</xm:f>
+            <xm:f>COUNTIF($C$52,Reference!$E$18)</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -4178,7 +4250,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>C44</xm:sqref>
+          <xm:sqref>C53</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="cellIs" priority="12" operator="lessThan" id="{19D8DF94-2AE3-467C-A57C-35B04CD0367F}">
@@ -4220,19 +4292,19 @@
           <x14:formula2>
             <xm:f>0</xm:f>
           </x14:formula2>
-          <xm:sqref>C43</xm:sqref>
+          <xm:sqref>C52</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2FD70BE5-C9FE-4FC2-BCF1-8C135E992CE5}">
           <x14:formula1>
             <xm:f>Reference!$E$33:$E$34</xm:f>
           </x14:formula1>
-          <xm:sqref>C45:D45</xm:sqref>
+          <xm:sqref>C54:D54</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{86E97738-BE4E-45D2-82E4-9BB20B6C5270}">
           <x14:formula1>
             <xm:f>Reference!$E$25:$E$30</xm:f>
           </x14:formula1>
-          <xm:sqref>C41:D41</xm:sqref>
+          <xm:sqref>C50:D50</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
@@ -4284,116 +4356,116 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="C1" s="34"/>
-      <c r="D1" s="123" t="s">
+      <c r="D1" s="125" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="125"/>
+      <c r="F1" s="125"/>
+      <c r="G1" s="56" t="s">
+        <v>369</v>
+      </c>
+      <c r="H1" s="126" t="s">
         <v>49</v>
       </c>
-      <c r="E1" s="123"/>
-      <c r="F1" s="123"/>
-      <c r="G1" s="56" t="s">
-        <v>374</v>
-      </c>
-      <c r="H1" s="124" t="s">
+      <c r="I1" s="126"/>
+      <c r="J1" s="126"/>
+      <c r="K1" s="126"/>
+      <c r="L1" s="127" t="s">
         <v>50</v>
       </c>
-      <c r="I1" s="124"/>
-      <c r="J1" s="124"/>
-      <c r="K1" s="124"/>
-      <c r="L1" s="125" t="s">
-        <v>51</v>
-      </c>
-      <c r="M1" s="125"/>
-      <c r="N1" s="125"/>
-      <c r="O1" s="125"/>
-      <c r="P1" s="125"/>
-      <c r="Q1" s="125"/>
-      <c r="R1" s="125"/>
-      <c r="S1" s="125"/>
-      <c r="T1" s="125"/>
-      <c r="U1" s="125"/>
-      <c r="V1" s="125"/>
-      <c r="W1" s="125"/>
-      <c r="X1" s="125"/>
-      <c r="Y1" s="125"/>
-      <c r="Z1" s="125"/>
+      <c r="M1" s="127"/>
+      <c r="N1" s="127"/>
+      <c r="O1" s="127"/>
+      <c r="P1" s="127"/>
+      <c r="Q1" s="127"/>
+      <c r="R1" s="127"/>
+      <c r="S1" s="127"/>
+      <c r="T1" s="127"/>
+      <c r="U1" s="127"/>
+      <c r="V1" s="127"/>
+      <c r="W1" s="127"/>
+      <c r="X1" s="127"/>
+      <c r="Y1" s="127"/>
+      <c r="Z1" s="127"/>
     </row>
     <row r="2" spans="1:26" s="10" customFormat="1" ht="95.4" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="75" t="s">
+        <v>305</v>
+      </c>
+      <c r="C2" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="75" t="s">
+      <c r="D2" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="57" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="57" t="s">
+        <v>353</v>
+      </c>
+      <c r="G2" s="58" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="59" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="59" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" s="59" t="s">
+        <v>58</v>
+      </c>
+      <c r="K2" s="59" t="s">
+        <v>59</v>
+      </c>
+      <c r="L2" s="60" t="s">
+        <v>60</v>
+      </c>
+      <c r="M2" s="60" t="s">
+        <v>309</v>
+      </c>
+      <c r="N2" s="60" t="s">
         <v>306</v>
       </c>
-      <c r="C2" s="36" t="s">
-        <v>53</v>
-      </c>
-      <c r="D2" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="57" t="s">
-        <v>55</v>
-      </c>
-      <c r="F2" s="57" t="s">
-        <v>358</v>
-      </c>
-      <c r="G2" s="58" t="s">
-        <v>56</v>
-      </c>
-      <c r="H2" s="59" t="s">
-        <v>57</v>
-      </c>
-      <c r="I2" s="59" t="s">
-        <v>58</v>
-      </c>
-      <c r="J2" s="59" t="s">
-        <v>59</v>
-      </c>
-      <c r="K2" s="59" t="s">
-        <v>60</v>
-      </c>
-      <c r="L2" s="60" t="s">
+      <c r="O2" s="60" t="s">
+        <v>307</v>
+      </c>
+      <c r="P2" s="60" t="s">
+        <v>308</v>
+      </c>
+      <c r="Q2" s="60" t="s">
+        <v>370</v>
+      </c>
+      <c r="R2" s="60" t="s">
+        <v>371</v>
+      </c>
+      <c r="S2" s="60" t="s">
+        <v>372</v>
+      </c>
+      <c r="T2" s="60" t="s">
+        <v>373</v>
+      </c>
+      <c r="U2" s="60" t="s">
+        <v>374</v>
+      </c>
+      <c r="V2" s="60" t="s">
+        <v>375</v>
+      </c>
+      <c r="W2" s="60" t="s">
+        <v>367</v>
+      </c>
+      <c r="X2" s="60" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y2" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="M2" s="60" t="s">
-        <v>310</v>
-      </c>
-      <c r="N2" s="60" t="s">
-        <v>307</v>
-      </c>
-      <c r="O2" s="60" t="s">
-        <v>308</v>
-      </c>
-      <c r="P2" s="60" t="s">
-        <v>309</v>
-      </c>
-      <c r="Q2" s="60" t="s">
-        <v>375</v>
-      </c>
-      <c r="R2" s="60" t="s">
-        <v>376</v>
-      </c>
-      <c r="S2" s="60" t="s">
-        <v>377</v>
-      </c>
-      <c r="T2" s="60" t="s">
-        <v>378</v>
-      </c>
-      <c r="U2" s="60" t="s">
-        <v>379</v>
-      </c>
-      <c r="V2" s="60" t="s">
-        <v>380</v>
-      </c>
-      <c r="W2" s="60" t="s">
-        <v>372</v>
-      </c>
-      <c r="X2" s="60" t="s">
-        <v>373</v>
-      </c>
-      <c r="Y2" s="60" t="s">
+      <c r="Z2" s="60" t="s">
         <v>62</v>
-      </c>
-      <c r="Z2" s="60" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -4405,7 +4477,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="39" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D3" s="39"/>
       <c r="E3" s="39"/>
@@ -4419,7 +4491,7 @@
         <v/>
       </c>
       <c r="L3" s="41" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M3" s="42" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -4484,7 +4556,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D4" s="26"/>
       <c r="E4" s="26"/>
@@ -4498,7 +4570,7 @@
         <v/>
       </c>
       <c r="L4" s="27" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M4" s="63" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -4563,7 +4635,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D5" s="26"/>
       <c r="E5" s="26"/>
@@ -4577,7 +4649,7 @@
         <v/>
       </c>
       <c r="L5" s="27" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M5" s="63" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -4642,7 +4714,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D6" s="26"/>
       <c r="E6" s="26"/>
@@ -4656,7 +4728,7 @@
         <v/>
       </c>
       <c r="L6" s="27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M6" s="63" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -4721,7 +4793,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D7" s="26"/>
       <c r="E7" s="26"/>
@@ -4735,7 +4807,7 @@
         <v/>
       </c>
       <c r="L7" s="27" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M7" s="63" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -4800,7 +4872,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D8" s="26"/>
       <c r="E8" s="26"/>
@@ -4814,7 +4886,7 @@
         <v/>
       </c>
       <c r="L8" s="27" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M8" s="63" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -4879,7 +4951,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D9" s="26"/>
       <c r="E9" s="26"/>
@@ -4893,7 +4965,7 @@
         <v/>
       </c>
       <c r="L9" s="27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M9" s="63" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -4958,7 +5030,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="50" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D10" s="50"/>
       <c r="E10" s="52"/>
@@ -4972,7 +5044,7 @@
         <v/>
       </c>
       <c r="L10" s="52" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M10" s="65" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -5037,7 +5109,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D11" s="13"/>
       <c r="E11" s="15"/>
@@ -5051,7 +5123,7 @@
         <v/>
       </c>
       <c r="L11" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M11" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -5116,7 +5188,7 @@
         <v>2</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D12" s="13"/>
       <c r="E12" s="15"/>
@@ -5130,7 +5202,7 @@
         <v/>
       </c>
       <c r="L12" s="27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M12" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -5195,7 +5267,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D13" s="13"/>
       <c r="E13" s="15"/>
@@ -5209,7 +5281,7 @@
         <v/>
       </c>
       <c r="L13" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M13" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -5274,7 +5346,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D14" s="13"/>
       <c r="E14" s="15"/>
@@ -5288,7 +5360,7 @@
         <v/>
       </c>
       <c r="L14" s="27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M14" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -5353,7 +5425,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D15" s="13"/>
       <c r="E15" s="15"/>
@@ -5367,7 +5439,7 @@
         <v/>
       </c>
       <c r="L15" s="27" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M15" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -5432,7 +5504,7 @@
         <v>2</v>
       </c>
       <c r="C16" s="33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D16" s="13"/>
       <c r="E16" s="15"/>
@@ -5446,7 +5518,7 @@
         <v/>
       </c>
       <c r="L16" s="27" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M16" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -5511,7 +5583,7 @@
         <v>2</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D17" s="13"/>
       <c r="E17" s="15"/>
@@ -5525,7 +5597,7 @@
         <v/>
       </c>
       <c r="L17" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M17" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -5590,7 +5662,7 @@
         <v>2</v>
       </c>
       <c r="C18" s="47" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D18" s="48"/>
       <c r="E18" s="49"/>
@@ -5604,7 +5676,7 @@
         <v/>
       </c>
       <c r="L18" s="52" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="M18" s="53" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -5669,7 +5741,7 @@
         <v>3</v>
       </c>
       <c r="C19" s="38" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D19" s="39"/>
       <c r="E19" s="41"/>
@@ -5683,7 +5755,7 @@
         <v/>
       </c>
       <c r="L19" s="41" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M19" s="42" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -5748,7 +5820,7 @@
         <v>3</v>
       </c>
       <c r="C20" s="33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D20" s="13"/>
       <c r="E20" s="15"/>
@@ -5762,7 +5834,7 @@
         <v/>
       </c>
       <c r="L20" s="27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="M20" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -5827,7 +5899,7 @@
         <v>3</v>
       </c>
       <c r="C21" s="33" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D21" s="13"/>
       <c r="E21" s="15"/>
@@ -5841,7 +5913,7 @@
         <v/>
       </c>
       <c r="L21" s="27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M21" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -5906,7 +5978,7 @@
         <v>3</v>
       </c>
       <c r="C22" s="32" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D22" s="13"/>
       <c r="E22" s="15"/>
@@ -5920,7 +5992,7 @@
         <v/>
       </c>
       <c r="L22" s="27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M22" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -5985,7 +6057,7 @@
         <v>3</v>
       </c>
       <c r="C23" s="32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D23" s="13"/>
       <c r="E23" s="15"/>
@@ -5999,7 +6071,7 @@
         <v/>
       </c>
       <c r="L23" s="27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M23" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -6064,7 +6136,7 @@
         <v>3</v>
       </c>
       <c r="C24" s="32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D24" s="13"/>
       <c r="E24" s="15"/>
@@ -6078,7 +6150,7 @@
         <v/>
       </c>
       <c r="L24" s="27" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M24" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -6143,7 +6215,7 @@
         <v>3</v>
       </c>
       <c r="C25" s="32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D25" s="13"/>
       <c r="E25" s="15"/>
@@ -6157,7 +6229,7 @@
         <v/>
       </c>
       <c r="L25" s="27" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M25" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -6222,7 +6294,7 @@
         <v>3</v>
       </c>
       <c r="C26" s="55" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D26" s="48"/>
       <c r="E26" s="49"/>
@@ -6236,7 +6308,7 @@
         <v/>
       </c>
       <c r="L26" s="52" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M26" s="53" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -6301,7 +6373,7 @@
         <v>4</v>
       </c>
       <c r="C27" s="38" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D27" s="39"/>
       <c r="E27" s="41"/>
@@ -6315,7 +6387,7 @@
         <v/>
       </c>
       <c r="L27" s="41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="M27" s="42" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -6380,7 +6452,7 @@
         <v>4</v>
       </c>
       <c r="C28" s="32" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D28" s="13"/>
       <c r="E28" s="15"/>
@@ -6394,7 +6466,7 @@
         <v/>
       </c>
       <c r="L28" s="27" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M28" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -6459,7 +6531,7 @@
         <v>4</v>
       </c>
       <c r="C29" s="32" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D29" s="13"/>
       <c r="E29" s="15"/>
@@ -6473,7 +6545,7 @@
         <v/>
       </c>
       <c r="L29" s="27" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M29" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -6538,7 +6610,7 @@
         <v>4</v>
       </c>
       <c r="C30" s="32" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D30" s="13"/>
       <c r="E30" s="15"/>
@@ -6552,7 +6624,7 @@
         <v/>
       </c>
       <c r="L30" s="27" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M30" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -6617,7 +6689,7 @@
         <v>4</v>
       </c>
       <c r="C31" s="32" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D31" s="13"/>
       <c r="E31" s="15"/>
@@ -6631,7 +6703,7 @@
         <v/>
       </c>
       <c r="L31" s="27" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M31" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -6696,7 +6768,7 @@
         <v>4</v>
       </c>
       <c r="C32" s="32" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D32" s="13"/>
       <c r="E32" s="15"/>
@@ -6710,7 +6782,7 @@
         <v/>
       </c>
       <c r="L32" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="M32" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -6775,7 +6847,7 @@
         <v>4</v>
       </c>
       <c r="C33" s="32" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D33" s="13"/>
       <c r="E33" s="15"/>
@@ -6789,7 +6861,7 @@
         <v/>
       </c>
       <c r="L33" s="27" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="M33" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -6854,7 +6926,7 @@
         <v>4</v>
       </c>
       <c r="C34" s="55" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D34" s="48"/>
       <c r="E34" s="49"/>
@@ -6868,7 +6940,7 @@
         <v/>
       </c>
       <c r="L34" s="52" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="M34" s="53" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -6933,7 +7005,7 @@
         <v>5</v>
       </c>
       <c r="C35" s="38" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D35" s="39"/>
       <c r="E35" s="41"/>
@@ -6947,7 +7019,7 @@
         <v/>
       </c>
       <c r="L35" s="41" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M35" s="42" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -7012,7 +7084,7 @@
         <v>5</v>
       </c>
       <c r="C36" s="32" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D36" s="13"/>
       <c r="E36" s="15"/>
@@ -7026,7 +7098,7 @@
         <v/>
       </c>
       <c r="L36" s="27" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M36" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -7091,7 +7163,7 @@
         <v>5</v>
       </c>
       <c r="C37" s="32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D37" s="13"/>
       <c r="E37" s="15"/>
@@ -7105,7 +7177,7 @@
         <v/>
       </c>
       <c r="L37" s="27" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="M37" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -7170,7 +7242,7 @@
         <v>5</v>
       </c>
       <c r="C38" s="32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D38" s="13"/>
       <c r="E38" s="15"/>
@@ -7184,7 +7256,7 @@
         <v/>
       </c>
       <c r="L38" s="27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M38" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -7249,7 +7321,7 @@
         <v>5</v>
       </c>
       <c r="C39" s="32" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D39" s="13"/>
       <c r="E39" s="15"/>
@@ -7263,7 +7335,7 @@
         <v/>
       </c>
       <c r="L39" s="27" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="M39" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -7328,7 +7400,7 @@
         <v>5</v>
       </c>
       <c r="C40" s="32" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D40" s="13"/>
       <c r="E40" s="15"/>
@@ -7342,7 +7414,7 @@
         <v/>
       </c>
       <c r="L40" s="27" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M40" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -7407,7 +7479,7 @@
         <v>5</v>
       </c>
       <c r="C41" s="32" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D41" s="13"/>
       <c r="E41" s="15"/>
@@ -7421,7 +7493,7 @@
         <v/>
       </c>
       <c r="L41" s="27" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M41" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -7486,7 +7558,7 @@
         <v>5</v>
       </c>
       <c r="C42" s="55" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D42" s="48"/>
       <c r="E42" s="49"/>
@@ -7500,7 +7572,7 @@
         <v/>
       </c>
       <c r="L42" s="52" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M42" s="53" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -7565,7 +7637,7 @@
         <v>6</v>
       </c>
       <c r="C43" s="38" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D43" s="39"/>
       <c r="E43" s="41"/>
@@ -7579,7 +7651,7 @@
         <v/>
       </c>
       <c r="L43" s="41" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M43" s="42" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -7644,7 +7716,7 @@
         <v>6</v>
       </c>
       <c r="C44" s="32" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D44" s="13"/>
       <c r="E44" s="15"/>
@@ -7658,7 +7730,7 @@
         <v/>
       </c>
       <c r="L44" s="27" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M44" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -7723,7 +7795,7 @@
         <v>6</v>
       </c>
       <c r="C45" s="32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D45" s="13"/>
       <c r="E45" s="15"/>
@@ -7737,7 +7809,7 @@
         <v/>
       </c>
       <c r="L45" s="27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="M45" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -7802,7 +7874,7 @@
         <v>6</v>
       </c>
       <c r="C46" s="32" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D46" s="13"/>
       <c r="E46" s="15"/>
@@ -7816,7 +7888,7 @@
         <v/>
       </c>
       <c r="L46" s="27" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="M46" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -7881,7 +7953,7 @@
         <v>6</v>
       </c>
       <c r="C47" s="32" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D47" s="13"/>
       <c r="E47" s="15"/>
@@ -7895,7 +7967,7 @@
         <v/>
       </c>
       <c r="L47" s="27" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="M47" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -7960,7 +8032,7 @@
         <v>6</v>
       </c>
       <c r="C48" s="32" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D48" s="13"/>
       <c r="E48" s="15"/>
@@ -7974,7 +8046,7 @@
         <v/>
       </c>
       <c r="L48" s="27" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="M48" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -8039,7 +8111,7 @@
         <v>6</v>
       </c>
       <c r="C49" s="32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D49" s="13"/>
       <c r="E49" s="15"/>
@@ -8053,7 +8125,7 @@
         <v/>
       </c>
       <c r="L49" s="27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="M49" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -8118,7 +8190,7 @@
         <v>6</v>
       </c>
       <c r="C50" s="55" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D50" s="48"/>
       <c r="E50" s="49"/>
@@ -8132,7 +8204,7 @@
         <v/>
       </c>
       <c r="L50" s="52" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="M50" s="53" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -8197,7 +8269,7 @@
         <v>7</v>
       </c>
       <c r="C51" s="38" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D51" s="39"/>
       <c r="E51" s="41"/>
@@ -8211,7 +8283,7 @@
         <v/>
       </c>
       <c r="L51" s="41" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="M51" s="42" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -8276,7 +8348,7 @@
         <v>7</v>
       </c>
       <c r="C52" s="32" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D52" s="13"/>
       <c r="E52" s="15"/>
@@ -8290,7 +8362,7 @@
         <v/>
       </c>
       <c r="L52" s="27" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M52" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -8355,7 +8427,7 @@
         <v>7</v>
       </c>
       <c r="C53" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D53" s="13"/>
       <c r="E53" s="15"/>
@@ -8369,7 +8441,7 @@
         <v/>
       </c>
       <c r="L53" s="27" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="M53" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -8434,7 +8506,7 @@
         <v>7</v>
       </c>
       <c r="C54" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D54" s="13"/>
       <c r="E54" s="15"/>
@@ -8448,7 +8520,7 @@
         <v/>
       </c>
       <c r="L54" s="27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M54" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -8513,7 +8585,7 @@
         <v>7</v>
       </c>
       <c r="C55" s="32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D55" s="13"/>
       <c r="E55" s="15"/>
@@ -8527,7 +8599,7 @@
         <v/>
       </c>
       <c r="L55" s="27" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M55" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -8592,7 +8664,7 @@
         <v>7</v>
       </c>
       <c r="C56" s="32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D56" s="13"/>
       <c r="E56" s="15"/>
@@ -8606,7 +8678,7 @@
         <v/>
       </c>
       <c r="L56" s="27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M56" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -8671,7 +8743,7 @@
         <v>7</v>
       </c>
       <c r="C57" s="32" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D57" s="13"/>
       <c r="E57" s="15"/>
@@ -8685,7 +8757,7 @@
         <v/>
       </c>
       <c r="L57" s="27" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M57" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -8750,7 +8822,7 @@
         <v>7</v>
       </c>
       <c r="C58" s="55" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D58" s="48"/>
       <c r="E58" s="49"/>
@@ -8764,7 +8836,7 @@
         <v/>
       </c>
       <c r="L58" s="52" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M58" s="53" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -8829,7 +8901,7 @@
         <v>8</v>
       </c>
       <c r="C59" s="38" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D59" s="39"/>
       <c r="E59" s="41"/>
@@ -8843,7 +8915,7 @@
         <v/>
       </c>
       <c r="L59" s="41" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M59" s="42" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -8908,7 +8980,7 @@
         <v>8</v>
       </c>
       <c r="C60" s="32" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D60" s="13"/>
       <c r="E60" s="15"/>
@@ -8922,7 +8994,7 @@
         <v/>
       </c>
       <c r="L60" s="27" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M60" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -8987,7 +9059,7 @@
         <v>8</v>
       </c>
       <c r="C61" s="32" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D61" s="13"/>
       <c r="E61" s="15"/>
@@ -9001,7 +9073,7 @@
         <v/>
       </c>
       <c r="L61" s="27" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M61" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -9066,7 +9138,7 @@
         <v>8</v>
       </c>
       <c r="C62" s="32" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D62" s="13"/>
       <c r="E62" s="15"/>
@@ -9080,7 +9152,7 @@
         <v/>
       </c>
       <c r="L62" s="27" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M62" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -9145,7 +9217,7 @@
         <v>8</v>
       </c>
       <c r="C63" s="32" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D63" s="13"/>
       <c r="E63" s="15"/>
@@ -9159,7 +9231,7 @@
         <v/>
       </c>
       <c r="L63" s="27" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M63" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -9224,7 +9296,7 @@
         <v>8</v>
       </c>
       <c r="C64" s="32" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D64" s="13"/>
       <c r="E64" s="15"/>
@@ -9238,7 +9310,7 @@
         <v/>
       </c>
       <c r="L64" s="27" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M64" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -9303,7 +9375,7 @@
         <v>8</v>
       </c>
       <c r="C65" s="32" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D65" s="13"/>
       <c r="E65" s="15"/>
@@ -9317,7 +9389,7 @@
         <v/>
       </c>
       <c r="L65" s="27" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M65" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -9382,7 +9454,7 @@
         <v>8</v>
       </c>
       <c r="C66" s="55" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D66" s="48"/>
       <c r="E66" s="49"/>
@@ -9396,7 +9468,7 @@
         <v/>
       </c>
       <c r="L66" s="52" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M66" s="53" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -9461,7 +9533,7 @@
         <v>9</v>
       </c>
       <c r="C67" s="38" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D67" s="39"/>
       <c r="E67" s="41"/>
@@ -9475,7 +9547,7 @@
         <v/>
       </c>
       <c r="L67" s="41" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="M67" s="42" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -9540,7 +9612,7 @@
         <v>9</v>
       </c>
       <c r="C68" s="32" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D68" s="13"/>
       <c r="E68" s="15"/>
@@ -9554,7 +9626,7 @@
         <v/>
       </c>
       <c r="L68" s="27" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="M68" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -9619,7 +9691,7 @@
         <v>9</v>
       </c>
       <c r="C69" s="32" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D69" s="13"/>
       <c r="E69" s="15"/>
@@ -9633,7 +9705,7 @@
         <v/>
       </c>
       <c r="L69" s="27" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="M69" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -9698,7 +9770,7 @@
         <v>9</v>
       </c>
       <c r="C70" s="32" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D70" s="13"/>
       <c r="E70" s="15"/>
@@ -9712,7 +9784,7 @@
         <v/>
       </c>
       <c r="L70" s="27" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M70" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -9777,7 +9849,7 @@
         <v>9</v>
       </c>
       <c r="C71" s="32" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D71" s="13"/>
       <c r="E71" s="15"/>
@@ -9791,7 +9863,7 @@
         <v/>
       </c>
       <c r="L71" s="27" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M71" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -9856,7 +9928,7 @@
         <v>9</v>
       </c>
       <c r="C72" s="32" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D72" s="13"/>
       <c r="E72" s="15"/>
@@ -9870,7 +9942,7 @@
         <v/>
       </c>
       <c r="L72" s="27" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M72" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -9935,7 +10007,7 @@
         <v>9</v>
       </c>
       <c r="C73" s="32" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D73" s="13"/>
       <c r="E73" s="15"/>
@@ -9949,7 +10021,7 @@
         <v/>
       </c>
       <c r="L73" s="27" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="M73" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -10014,7 +10086,7 @@
         <v>9</v>
       </c>
       <c r="C74" s="55" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D74" s="48"/>
       <c r="E74" s="49"/>
@@ -10028,7 +10100,7 @@
         <v/>
       </c>
       <c r="L74" s="52" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="M74" s="53" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -10093,7 +10165,7 @@
         <v>10</v>
       </c>
       <c r="C75" s="38" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D75" s="39"/>
       <c r="E75" s="41"/>
@@ -10107,7 +10179,7 @@
         <v/>
       </c>
       <c r="L75" s="41" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M75" s="42" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -10172,7 +10244,7 @@
         <v>10</v>
       </c>
       <c r="C76" s="32" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D76" s="13"/>
       <c r="E76" s="15"/>
@@ -10186,7 +10258,7 @@
         <v/>
       </c>
       <c r="L76" s="27" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="M76" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -10251,7 +10323,7 @@
         <v>10</v>
       </c>
       <c r="C77" s="32" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D77" s="13"/>
       <c r="E77" s="15"/>
@@ -10265,7 +10337,7 @@
         <v/>
       </c>
       <c r="L77" s="27" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="M77" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -10330,7 +10402,7 @@
         <v>10</v>
       </c>
       <c r="C78" s="32" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D78" s="13"/>
       <c r="E78" s="15"/>
@@ -10344,7 +10416,7 @@
         <v/>
       </c>
       <c r="L78" s="27" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="M78" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -10409,7 +10481,7 @@
         <v>10</v>
       </c>
       <c r="C79" s="32" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D79" s="13"/>
       <c r="E79" s="15"/>
@@ -10423,7 +10495,7 @@
         <v/>
       </c>
       <c r="L79" s="27" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="M79" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -10488,7 +10560,7 @@
         <v>10</v>
       </c>
       <c r="C80" s="32" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D80" s="13"/>
       <c r="E80" s="15"/>
@@ -10502,7 +10574,7 @@
         <v/>
       </c>
       <c r="L80" s="27" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="M80" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -10567,7 +10639,7 @@
         <v>10</v>
       </c>
       <c r="C81" s="32" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D81" s="13"/>
       <c r="E81" s="15"/>
@@ -10581,7 +10653,7 @@
         <v/>
       </c>
       <c r="L81" s="27" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="M81" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -10646,7 +10718,7 @@
         <v>10</v>
       </c>
       <c r="C82" s="55" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D82" s="48"/>
       <c r="E82" s="49"/>
@@ -10660,7 +10732,7 @@
         <v/>
       </c>
       <c r="L82" s="52" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M82" s="53" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -10725,7 +10797,7 @@
         <v>11</v>
       </c>
       <c r="C83" s="38" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D83" s="39"/>
       <c r="E83" s="41"/>
@@ -10739,7 +10811,7 @@
         <v/>
       </c>
       <c r="L83" s="41" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="M83" s="42" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -10804,7 +10876,7 @@
         <v>11</v>
       </c>
       <c r="C84" s="32" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D84" s="13"/>
       <c r="E84" s="15"/>
@@ -10818,7 +10890,7 @@
         <v/>
       </c>
       <c r="L84" s="27" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M84" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -10883,7 +10955,7 @@
         <v>11</v>
       </c>
       <c r="C85" s="32" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D85" s="13"/>
       <c r="E85" s="15"/>
@@ -10897,7 +10969,7 @@
         <v/>
       </c>
       <c r="L85" s="27" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="M85" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -10962,7 +11034,7 @@
         <v>11</v>
       </c>
       <c r="C86" s="32" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D86" s="13"/>
       <c r="E86" s="15"/>
@@ -10976,7 +11048,7 @@
         <v/>
       </c>
       <c r="L86" s="27" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M86" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -11041,7 +11113,7 @@
         <v>11</v>
       </c>
       <c r="C87" s="32" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D87" s="13"/>
       <c r="E87" s="15"/>
@@ -11055,7 +11127,7 @@
         <v/>
       </c>
       <c r="L87" s="27" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M87" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -11120,7 +11192,7 @@
         <v>11</v>
       </c>
       <c r="C88" s="32" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D88" s="13"/>
       <c r="E88" s="15"/>
@@ -11134,7 +11206,7 @@
         <v/>
       </c>
       <c r="L88" s="27" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="M88" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -11199,7 +11271,7 @@
         <v>11</v>
       </c>
       <c r="C89" s="32" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D89" s="13"/>
       <c r="E89" s="15"/>
@@ -11213,7 +11285,7 @@
         <v/>
       </c>
       <c r="L89" s="27" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M89" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -11278,7 +11350,7 @@
         <v>11</v>
       </c>
       <c r="C90" s="55" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D90" s="48"/>
       <c r="E90" s="49"/>
@@ -11292,7 +11364,7 @@
         <v/>
       </c>
       <c r="L90" s="52" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="M90" s="53" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -11357,7 +11429,7 @@
         <v>12</v>
       </c>
       <c r="C91" s="38" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D91" s="39"/>
       <c r="E91" s="41"/>
@@ -11371,7 +11443,7 @@
         <v/>
       </c>
       <c r="L91" s="41" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="M91" s="42" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -11436,7 +11508,7 @@
         <v>12</v>
       </c>
       <c r="C92" s="32" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D92" s="13"/>
       <c r="E92" s="15"/>
@@ -11450,7 +11522,7 @@
         <v/>
       </c>
       <c r="L92" s="27" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="M92" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -11515,7 +11587,7 @@
         <v>12</v>
       </c>
       <c r="C93" s="32" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D93" s="13"/>
       <c r="E93" s="15"/>
@@ -11529,7 +11601,7 @@
         <v/>
       </c>
       <c r="L93" s="27" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="M93" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -11594,7 +11666,7 @@
         <v>12</v>
       </c>
       <c r="C94" s="32" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D94" s="13"/>
       <c r="E94" s="15"/>
@@ -11608,7 +11680,7 @@
         <v/>
       </c>
       <c r="L94" s="27" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="M94" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -11673,7 +11745,7 @@
         <v>12</v>
       </c>
       <c r="C95" s="32" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D95" s="13"/>
       <c r="E95" s="15"/>
@@ -11687,7 +11759,7 @@
         <v/>
       </c>
       <c r="L95" s="27" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="M95" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -11752,7 +11824,7 @@
         <v>12</v>
       </c>
       <c r="C96" s="32" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D96" s="13"/>
       <c r="E96" s="15"/>
@@ -11766,7 +11838,7 @@
         <v/>
       </c>
       <c r="L96" s="27" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="M96" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -11831,7 +11903,7 @@
         <v>12</v>
       </c>
       <c r="C97" s="32" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D97" s="13"/>
       <c r="E97" s="15"/>
@@ -11845,7 +11917,7 @@
         <v/>
       </c>
       <c r="L97" s="27" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M97" s="31" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -11910,7 +11982,7 @@
         <v>12</v>
       </c>
       <c r="C98" s="55" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D98" s="48"/>
       <c r="E98" s="49"/>
@@ -11924,7 +11996,7 @@
         <v/>
       </c>
       <c r="L98" s="52" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="M98" s="53" t="str">
         <f>IF(LEN(tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]])=0,"",IF(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]&gt;endrepair_maxvol,endrepair_maxvol,ROUNDUP(SUM(pcr_product_targetmass_per_sample/tbl_SeqLib[[#This Row],[PCR '[DNA'] (ng / µl)]]),1)))</f>
@@ -12191,7 +12263,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="46.2" x14ac:dyDescent="0.85">
       <c r="A1" s="29" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B1" s="88"/>
       <c r="C1" s="88"/>
@@ -12208,7 +12280,7 @@
     </row>
     <row r="2" spans="1:13" ht="33.6" x14ac:dyDescent="0.65">
       <c r="A2" s="86" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="B2" s="88"/>
       <c r="C2" s="88"/>
@@ -12225,7 +12297,7 @@
     </row>
     <row r="3" spans="1:13" ht="33.6" x14ac:dyDescent="0.65">
       <c r="A3" s="86" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="B3" s="88"/>
       <c r="C3" s="88"/>
@@ -12257,7 +12329,7 @@
     </row>
     <row r="5" spans="1:13" ht="33.6" x14ac:dyDescent="0.65">
       <c r="A5" s="87" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B5" s="88"/>
       <c r="C5" s="88"/>
@@ -12274,7 +12346,7 @@
     </row>
     <row r="6" spans="1:13" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A6" s="30" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="B6" s="88"/>
       <c r="C6" s="88"/>
@@ -12291,7 +12363,7 @@
     </row>
     <row r="7" spans="1:13" ht="33.6" x14ac:dyDescent="0.65">
       <c r="A7" s="85" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="B7" s="88"/>
       <c r="C7" s="88"/>
@@ -12308,7 +12380,7 @@
     </row>
     <row r="8" spans="1:13" ht="33.6" x14ac:dyDescent="0.65">
       <c r="A8" s="86" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="B8" s="88"/>
       <c r="C8" s="88"/>
@@ -12325,123 +12397,123 @@
     </row>
     <row r="14" spans="1:13" ht="46.2" x14ac:dyDescent="0.85">
       <c r="A14" s="29" t="s">
-        <v>384</v>
+        <v>379</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A15" s="18" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
       <c r="E15" s="18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F15" s="18"/>
       <c r="I15" s="18" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="20" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B16" s="21"/>
       <c r="C16" s="21"/>
       <c r="E16" s="21" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F16" s="67"/>
       <c r="I16" s="90" t="s">
+        <v>260</v>
+      </c>
+      <c r="J16" s="90" t="s">
         <v>261</v>
       </c>
-      <c r="J16" s="90" t="s">
+      <c r="L16" s="90" t="s">
         <v>262</v>
-      </c>
-      <c r="L16" s="90" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="B17">
         <v>15</v>
       </c>
       <c r="C17" s="82" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="D17" s="19"/>
       <c r="E17" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I17" s="34" t="s">
+        <v>327</v>
+      </c>
+      <c r="J17" s="34" t="s">
         <v>328</v>
       </c>
-      <c r="J17" s="34" t="s">
-        <v>329</v>
-      </c>
       <c r="L17" s="34" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B18" s="34">
         <v>200</v>
       </c>
       <c r="C18" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D18" s="19"/>
       <c r="E18" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I18" s="34" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="J18" s="34" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="L18" s="34" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B19" s="34">
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I19" s="34" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="J19" s="34" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="L19" s="34" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B20" s="34">
         <v>800</v>
       </c>
       <c r="C20" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F20" s="67"/>
       <c r="I20" s="34"/>
@@ -12450,13 +12522,13 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="B21" s="34">
         <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E21">
         <v>100</v>
@@ -12467,13 +12539,13 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B22" s="34">
         <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E22">
         <v>50</v>
@@ -12484,14 +12556,14 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="B23">
         <f>ROUND(SUM(flowcell_targetmass/flowcell_maxvol),0)</f>
         <v>73</v>
       </c>
       <c r="C23" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="I23" s="34"/>
       <c r="J23" s="34"/>
@@ -12499,16 +12571,16 @@
     </row>
     <row r="24" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B24" s="35" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C24" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F24" s="67"/>
       <c r="I24" s="34"/>
@@ -12517,7 +12589,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I25" s="34"/>
       <c r="J25" s="34"/>
@@ -12525,12 +12597,12 @@
     </row>
     <row r="26" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="20" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B26" s="21"/>
       <c r="C26" s="21"/>
       <c r="E26" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="I26" s="34"/>
       <c r="J26" s="34"/>
@@ -12542,183 +12614,183 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="B27" t="s">
         <v>269</v>
       </c>
-      <c r="B27" t="s">
-        <v>270</v>
-      </c>
       <c r="E27" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="I27" s="22"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B28" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E28" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I28" s="22"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B29">
         <v>10</v>
       </c>
       <c r="E29" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="I29" s="22"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E30" s="10" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F30" s="10"/>
       <c r="I30" s="22"/>
     </row>
     <row r="31" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="20" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I31" s="22"/>
     </row>
     <row r="32" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="10" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="E32" s="21" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F32" s="67"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="E33" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G33" s="10"/>
       <c r="H33" s="10"/>
     </row>
     <row r="34" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E36" s="68" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F36" s="67"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E37" s="67" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F37" s="67" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E38" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F38" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E39" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F39" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E40" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F40" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E41" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="F41" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I41" s="10"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E42" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F42" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J42" s="10"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E43" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F43" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E44" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F44" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E47" s="21" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F47" s="67"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E48" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="49" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E49" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="51" spans="5:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E51" s="74" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
     </row>
     <row r="52" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E52" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
     </row>
     <row r="53" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E53" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
     </row>
     <row r="54" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E54" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -12763,70 +12835,70 @@
   <sheetData>
     <row r="1" spans="1:22" s="10" customFormat="1" ht="78" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>272</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="C1" s="10" t="s">
         <v>273</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="10" t="s">
+        <v>344</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>275</v>
       </c>
-      <c r="E1" s="10" t="s">
-        <v>346</v>
-      </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>276</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>277</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>278</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="J1" s="10" t="s">
+        <v>339</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="L1" s="10" t="s">
         <v>279</v>
       </c>
-      <c r="J1" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>344</v>
-      </c>
-      <c r="L1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>280</v>
       </c>
-      <c r="M1" s="10" t="s">
+      <c r="N1" s="10" t="s">
         <v>281</v>
       </c>
-      <c r="N1" s="10" t="s">
+      <c r="O1" s="10" t="s">
+        <v>365</v>
+      </c>
+      <c r="P1" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="O1" s="10" t="s">
-        <v>370</v>
-      </c>
-      <c r="P1" s="10" t="s">
+      <c r="Q1" s="10" t="s">
         <v>283</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="R1" s="10" t="s">
         <v>284</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="S1" s="10" t="s">
         <v>285</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="T1" s="10" t="s">
         <v>286</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="U1" s="10" t="s">
         <v>287</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="V1" s="10" t="s">
         <v>288</v>
-      </c>
-      <c r="V1" s="10" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.3">
@@ -12873,9 +12945,9 @@
         <f>IF(LEN(endrepair_maxvol)=0,"",endrepair_maxvol)</f>
         <v>10</v>
       </c>
-      <c r="L2" t="str">
+      <c r="L2">
         <f>IF(DNAconc_pooled=0,"",DNAconc_pooled)</f>
-        <v/>
+        <v>146</v>
       </c>
       <c r="M2" t="str">
         <f>IF(LEN(seq_platform)=0,"",seq_platform)</f>
@@ -12885,9 +12957,9 @@
         <f>IF(LEN(flowcell_targetmass)=0,"",flowcell_targetmass)</f>
         <v>800</v>
       </c>
-      <c r="O2" t="str">
+      <c r="O2">
         <f>IFERROR(SUM(adaptlig_rxn_vol*DNAconc_pooled), "")</f>
-        <v/>
+        <v>803</v>
       </c>
       <c r="P2">
         <f>IF(LEN(flowcell_maxvol)=0,"",flowcell_maxvol)</f>
@@ -12905,9 +12977,9 @@
         <f>IF(LEN(flowcell_status)=0,"",flowcell_status)</f>
         <v/>
       </c>
-      <c r="T2" t="str">
+      <c r="T2">
         <f>IF(LEN(flowcell_checkpores)=0,"",flowcell_checkpores)</f>
-        <v/>
+        <v>234</v>
       </c>
       <c r="U2" t="str">
         <f>IF(LEN(flowcell_runduration)=0,"",flowcell_runduration)</f>
@@ -12951,31 +13023,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B1" t="s">
         <v>290</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>354</v>
+      </c>
+      <c r="D1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E1" t="s">
         <v>291</v>
       </c>
-      <c r="C1" t="s">
-        <v>359</v>
-      </c>
-      <c r="D1" t="s">
-        <v>272</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>292</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>293</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>294</v>
       </c>
-      <c r="H1" t="s">
-        <v>295</v>
-      </c>
       <c r="I1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated version and handling of filepaths without an expid identified
</commit_message>
<xml_diff>
--- a/templates/NOMADS_Library_Rapid_Worksheet.xlsx
+++ b/templates/NOMADS_Library_Rapid_Worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\git\warehouse\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4371B737-9FC6-486F-BD09-256DD287924A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{154BEE54-E7BD-45DD-ADE3-68FAFD44631D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="27288" windowHeight="17532" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Assay" sheetId="1" r:id="rId1"/>
     <sheet name="Library" sheetId="2" r:id="rId2"/>
     <sheet name="Reference" sheetId="4" r:id="rId3"/>
-    <sheet name="expt_metadata" sheetId="5" state="hidden" r:id="rId4"/>
+    <sheet name="expt_metadata" sheetId="5" r:id="rId4"/>
     <sheet name="rxn_metadata" sheetId="6" state="hidden" r:id="rId5"/>
   </sheets>
   <definedNames>
@@ -93,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="411" uniqueCount="396">
   <si>
     <t>Date:</t>
   </si>
@@ -1315,9 +1315,6 @@
   </si>
   <si>
     <t>PCR product (µl) to add (2 per plate)</t>
-  </si>
-  <si>
-    <t>Hidden swga / pcr / seqlib identifiers</t>
   </si>
   <si>
     <t>Mk1d</t>
@@ -1420,12 +1417,6 @@
     <t>This template is to be used to record library prep and sequencing steps as part of a NOMADS sequencing run.</t>
   </si>
   <si>
-    <t>Hidden additional tabs</t>
-  </si>
-  <si>
-    <t>Combined Instructions into Reference sheet</t>
-  </si>
-  <si>
     <t>Volume to adaptor ligate (µl)</t>
   </si>
   <si>
@@ -1460,6 +1451,9 @@
   </si>
   <si>
     <t>In minknow select 'SQK-RBK114-96' kit with 'Super accurate basecalling'</t>
+  </si>
+  <si>
+    <t>Added protcol details to list</t>
   </si>
 </sst>
 </file>
@@ -3522,7 +3516,7 @@
   </sheetPr>
   <dimension ref="A1:Q55"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
@@ -3895,11 +3889,11 @@
       </c>
       <c r="E26" s="115"/>
       <c r="F26" s="118" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="G26" s="118"/>
       <c r="H26" s="118" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="I26" s="118"/>
     </row>
@@ -3935,7 +3929,7 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -3960,7 +3954,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="6" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
@@ -3976,27 +3970,27 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4049,7 +4043,7 @@
     </row>
     <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="8" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="B46" s="91"/>
       <c r="C46" s="91"/>
@@ -4059,13 +4053,13 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="6" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C48" s="4"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="92" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C49" s="4"/>
     </row>
@@ -12276,7 +12270,7 @@
     </row>
     <row r="2" spans="1:13" ht="33.6" x14ac:dyDescent="0.65">
       <c r="A2" s="86" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B2" s="88"/>
       <c r="C2" s="88"/>
@@ -12293,7 +12287,7 @@
     </row>
     <row r="3" spans="1:13" ht="33.6" x14ac:dyDescent="0.65">
       <c r="A3" s="86" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B3" s="88"/>
       <c r="C3" s="88"/>
@@ -12342,7 +12336,7 @@
     </row>
     <row r="6" spans="1:13" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A6" s="30" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B6" s="88"/>
       <c r="C6" s="88"/>
@@ -12359,7 +12353,7 @@
     </row>
     <row r="7" spans="1:13" ht="33.6" x14ac:dyDescent="0.65">
       <c r="A7" s="85" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B7" s="88"/>
       <c r="C7" s="88"/>
@@ -12376,7 +12370,7 @@
     </row>
     <row r="8" spans="1:13" ht="33.6" x14ac:dyDescent="0.65">
       <c r="A8" s="86" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B8" s="88"/>
       <c r="C8" s="88"/>
@@ -12393,7 +12387,7 @@
     </row>
     <row r="14" spans="1:13" ht="46.2" x14ac:dyDescent="0.85">
       <c r="A14" s="29" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="18" x14ac:dyDescent="0.35">
@@ -12616,7 +12610,7 @@
         <v>269</v>
       </c>
       <c r="E27" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="I27" s="22"/>
     </row>
@@ -12637,7 +12631,7 @@
         <v>270</v>
       </c>
       <c r="B29">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E29" t="s">
         <v>302</v>
@@ -12659,7 +12653,7 @@
     </row>
     <row r="32" spans="1:17" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="10" t="s">
-        <v>376</v>
+        <v>395</v>
       </c>
       <c r="E32" s="21" t="s">
         <v>304</v>
@@ -12667,19 +12661,15 @@
       <c r="F32" s="67"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A33" s="10" t="s">
-        <v>384</v>
-      </c>
+      <c r="A33" s="10"/>
       <c r="E33" t="s">
         <v>43</v>
       </c>
       <c r="G33" s="10"/>
       <c r="H33" s="10"/>
     </row>
-    <row r="34" spans="1:10" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A34" s="10" t="s">
-        <v>385</v>
-      </c>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="10"/>
     </row>
     <row r="36" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E36" s="68" t="s">
@@ -12790,7 +12780,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <protectedRanges>
     <protectedRange sqref="L17:L26" name="projectlist"/>
     <protectedRange sqref="I17:J26" name="personlist"/>
@@ -12920,7 +12909,7 @@
       </c>
       <c r="F2">
         <f>IF(LEN(exp_version)=0,"",exp_version)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" t="str">
         <f>IF(LEN(exp_notes)=0,"",exp_notes)</f>

</xml_diff>